<commit_message>
Auto commit - 09011812
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$14</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-01  )</t>
   </si>
@@ -220,6 +220,109 @@
     <t>O</t>
   </si>
   <si>
+    <t>E4917114082902</t>
+  </si>
+  <si>
+    <t>板橋翠華店</t>
+  </si>
+  <si>
+    <t>新北市板橋區</t>
+  </si>
+  <si>
+    <t>2025-08-29 21:22:17</t>
+  </si>
+  <si>
+    <t>夜間</t>
+  </si>
+  <si>
+    <t>HLD3</t>
+  </si>
+  <si>
+    <t>HL-熱感發票機</t>
+  </si>
+  <si>
+    <t>D304</t>
+  </si>
+  <si>
+    <t>空白列印/印一半/未列印</t>
+  </si>
+  <si>
+    <t>TM1熱感發票機(BSC10II)門市店長反應8/5台芝來更換錢箱控制線接主機位置後，有一個多禮拜發票印都是正常的，但從8/27開始，交班後第一筆未出發票或是清帳後未印出退瓶帳條，都是出現像卡紙的聲音後，後續出一小截的空白紙，確認當下TM都沒有出現錯誤訊息，發票機也沒有異常燈號顯示，但此情況已造成門市作業不便........還請台芝到店協助(8/29.1300清帳交班後1500開班第一筆交易發票完全未印出.)</t>
+  </si>
+  <si>
+    <t>THILF04917</t>
+  </si>
+  <si>
+    <t>狄澤洋</t>
+  </si>
+  <si>
+    <t>2025-08-29 21:37:13</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 15:35:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 01:37:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上：8155006322
+換下：8155004438</t>
+  </si>
+  <si>
+    <t>13652114082901</t>
+  </si>
+  <si>
+    <t>北縣莊民店</t>
+  </si>
+  <si>
+    <t>新北市新莊區</t>
+  </si>
+  <si>
+    <t>2025-08-29 21:37:46</t>
+  </si>
+  <si>
+    <t>HLF2</t>
+  </si>
+  <si>
+    <t>HL-CCD掃描器(TM)</t>
+  </si>
+  <si>
+    <t>F201</t>
+  </si>
+  <si>
+    <t>掃描無反應或感應不良</t>
+  </si>
+  <si>
+    <t>門市反應TM1 CCD掃描器(HC56II-TR、HC76-TR)膠條破掉，要求協助更換......還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03652</t>
+  </si>
+  <si>
+    <t>湯家瑋</t>
+  </si>
+  <si>
+    <t>2025-08-29 21:40:13</t>
+  </si>
+  <si>
+    <t>2025-09-01 17:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 17:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 01:40:00</t>
+  </si>
+  <si>
+    <t>更換手持
+換上8119012887
+換下8119006676</t>
+  </si>
+  <si>
     <t>E2543114083001</t>
   </si>
   <si>
@@ -273,6 +376,47 @@
 換上8183000272</t>
   </si>
   <si>
+    <t>1D111114083102</t>
+  </si>
+  <si>
+    <t>D111</t>
+  </si>
+  <si>
+    <t>北縣府中店</t>
+  </si>
+  <si>
+    <t>2025-08-31 10:06:40</t>
+  </si>
+  <si>
+    <t>星期日</t>
+  </si>
+  <si>
+    <t>上午</t>
+  </si>
+  <si>
+    <t>觸控不良(游標偏移)</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)游標會亂跑，未點選螢幕卻一直發出逼逼的聲音，客服已協助執行觸控校正仍異常，與門市確認螢幕無貼保護貼、文宣...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D111</t>
+  </si>
+  <si>
+    <t>2025-08-31 10:08:19</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:12:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:45:00</t>
+  </si>
+  <si>
+    <t>更換TCx800主機
+換上：8185000056
+換下：8185002301</t>
+  </si>
+  <si>
     <t>服務</t>
   </si>
   <si>
@@ -285,9 +429,6 @@
     <t>THILF03921</t>
   </si>
   <si>
-    <t>湯家瑋</t>
-  </si>
-  <si>
     <t>2025-09-01 11:55:09</t>
   </si>
   <si>
@@ -295,6 +436,102 @@
   </si>
   <si>
     <t>PMQ3</t>
+  </si>
+  <si>
+    <t>五股工商店</t>
+  </si>
+  <si>
+    <t>THILF04316</t>
+  </si>
+  <si>
+    <t>2025-09-01 13:53:54</t>
+  </si>
+  <si>
+    <t>2025-09-01 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 13:50:00</t>
+  </si>
+  <si>
+    <t>三重福仁店</t>
+  </si>
+  <si>
+    <t>THILF03957</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:37:52</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:15:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:35:00</t>
+  </si>
+  <si>
+    <t>L517</t>
+  </si>
+  <si>
+    <t>車麗屋蘆洲店</t>
+  </si>
+  <si>
+    <t>THILF0L517</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:49:28</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:33:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 14:50:00</t>
+  </si>
+  <si>
+    <t>蘆洲鷺江店</t>
+  </si>
+  <si>
+    <t>THILF02890</t>
+  </si>
+  <si>
+    <t>2025-09-01 15:43:48</t>
+  </si>
+  <si>
+    <t>2025-09-01 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 15:43:00</t>
+  </si>
+  <si>
+    <t>D193</t>
+  </si>
+  <si>
+    <t>蘆洲權義店</t>
+  </si>
+  <si>
+    <t>THILF0D193</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:15:04</t>
+  </si>
+  <si>
+    <t>2025-09-01 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:10:00</t>
+  </si>
+  <si>
+    <t>蘆洲鴻悅店</t>
+  </si>
+  <si>
+    <t>THILF05197</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:39:02</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-01 16:40:00</t>
   </si>
 </sst>
 </file>
@@ -708,10 +945,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AK14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1014,7 +1251,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="3">
-        <v>2025083749</v>
+        <v>2025083747</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>61</v>
@@ -1023,7 +1260,7 @@
         <v>40</v>
       </c>
       <c r="F4" s="3">
-        <v>2543</v>
+        <v>4917</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>62</v>
@@ -1035,34 +1272,34 @@
         <v>64</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="Q4" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T4" s="3">
         <v>1</v>
@@ -1083,7 +1320,7 @@
         <v>76</v>
       </c>
       <c r="Z4" s="3">
-        <v>0.5</v>
+        <v>1.1</v>
       </c>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3" t="s">
@@ -1108,15 +1345,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2025083748</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="7">
-        <v>2025090198</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F5" s="7">
-        <v>3921</v>
+        <v>3652</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>79</v>
@@ -1124,22 +1365,38 @@
       <c r="H5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="I5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="Q5" s="7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="R5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="T5" s="7">
         <v>1</v>
@@ -1148,28 +1405,28 @@
         <v>53</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y5" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="Z5" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA5" s="7"/>
       <c r="AB5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD5" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC5" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
       <c r="AF5" s="7"/>
       <c r="AG5" s="7"/>
@@ -1177,6 +1434,739 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
       <c r="AK5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2025083749</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2543</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2025083764</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="7">
+        <v>1</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2025090198</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>3921</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2025090208</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7">
+        <v>4316</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T9" s="7">
+        <v>1</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2025090217</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>3957</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2025090222</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T11" s="7">
+        <v>1</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2025090282</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>2890</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="3">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2025090290</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="7">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2025090294</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>5197</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09021117
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$18</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-01  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-02  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -417,6 +417,39 @@
 換下：8185002301</t>
   </si>
   <si>
+    <t>13752114090101</t>
+  </si>
+  <si>
+    <t>板橋豫章店</t>
+  </si>
+  <si>
+    <t>2025-09-01 09:12:32</t>
+  </si>
+  <si>
+    <t>星期一</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控都沒反應且畫面跳到愛心畫面，VNC查看門市觸控異常鼠標飄移亂點無法操作觸控校正，門市已自行重啟多次仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03752</t>
+  </si>
+  <si>
+    <t>2025-09-01 09:15:25</t>
+  </si>
+  <si>
+    <t>2025-09-02 09:17:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 09:47:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 13:15:00</t>
+  </si>
+  <si>
+    <t>一般轉緊急</t>
+  </si>
+  <si>
     <t>服務</t>
   </si>
   <si>
@@ -532,6 +565,77 @@
   </si>
   <si>
     <t>2025-09-01 16:40:00</t>
+  </si>
+  <si>
+    <t>13752114090102</t>
+  </si>
+  <si>
+    <t>急修件</t>
+  </si>
+  <si>
+    <t>2025-09-01 17:08:49</t>
+  </si>
+  <si>
+    <t>2025/09/01 17:05總公司明翰來電啟動緊急叫修:門市反應TM2(TCX800)觸控都沒反應且畫面跳到愛心畫面，VNC查看門市觸控異常鼠標飄移亂點無法操作觸控校正，門市已自行重啟多次仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-01 17:09:54</t>
+  </si>
+  <si>
+    <t>2025-09-02 08:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 09:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 10:09:00</t>
+  </si>
+  <si>
+    <t>更換TCx800主機（硬碟無更換）
+換上：8185000114
+換下：8185002487</t>
+  </si>
+  <si>
+    <t>E2224114090201</t>
+  </si>
+  <si>
+    <t>板橋莒光店</t>
+  </si>
+  <si>
+    <t>2025-09-02 07:36:24</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>無電源反應、無法開機</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)點選版更後就黑畫面無法開機，電源燈無亮燈，門市告知後方線路雜亂無法協助客服拔插，ping80不通無法vnc...請台芝到店協助(機1按完版本更新就無畫面) 已與門市確認09/02交易資料PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)(版本更新後都沒有開機)</t>
+  </si>
+  <si>
+    <t>THILF02224</t>
+  </si>
+  <si>
+    <t>2025-09-02 09:07:27</t>
+  </si>
+  <si>
+    <t>2025-09-02 09:22:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 09:52:00</t>
+  </si>
+  <si>
+    <t>2025-09-03 13:07:00</t>
+  </si>
+  <si>
+    <t>取消報修</t>
+  </si>
+  <si>
+    <t>2025-09-02 10:21:49</t>
+  </si>
+  <si>
+    <t>2025-09-02 10:20:00</t>
   </si>
 </sst>
 </file>
@@ -945,10 +1049,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK14"/>
+  <dimension ref="A1:AK18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC11" sqref="AC11"/>
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1636,38 +1740,58 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2025090012</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="3">
-        <v>2025090198</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F8" s="3">
-        <v>3921</v>
+        <v>3752</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>125</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="10"/>
+      <c r="J8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="Q8" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="T8" s="3">
         <v>1</v>
@@ -1676,15 +1800,17 @@
         <v>53</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y8" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="Z8" s="3">
         <v>0.5</v>
       </c>
@@ -1693,11 +1819,9 @@
         <v>58</v>
       </c>
       <c r="AC8" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD8" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
@@ -1713,21 +1837,21 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C9" s="7">
-        <v>2025090208</v>
+        <v>2025090198</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7">
-        <v>4316</v>
+        <v>3921</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1738,7 +1862,7 @@
       <c r="O9" s="8"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="7" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>51</v>
@@ -1753,24 +1877,24 @@
         <v>53</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC9" s="9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>60</v>
@@ -1790,21 +1914,21 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C10" s="3">
-        <v>2025090217</v>
+        <v>2025090208</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3">
-        <v>3957</v>
+        <v>4316</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1815,13 +1939,13 @@
       <c r="O10" s="4"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="T10" s="3">
         <v>1</v>
@@ -1830,13 +1954,13 @@
         <v>53</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3">
@@ -1847,7 +1971,7 @@
         <v>58</v>
       </c>
       <c r="AC10" s="10" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AD10" s="3" t="s">
         <v>60</v>
@@ -1867,21 +1991,21 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C11" s="7">
-        <v>2025090222</v>
+        <v>2025090217</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
-        <v>141</v>
+      <c r="F11" s="7">
+        <v>3957</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1892,7 +2016,7 @@
       <c r="O11" s="8"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="7" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>51</v>
@@ -1907,13 +2031,13 @@
         <v>53</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7">
@@ -1924,7 +2048,7 @@
         <v>58</v>
       </c>
       <c r="AC11" s="9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>60</v>
@@ -1944,18 +2068,18 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C12" s="3">
-        <v>2025090282</v>
+        <v>2025090222</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3">
-        <v>2890</v>
+      <c r="F12" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>42</v>
@@ -1969,7 +2093,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>51</v>
@@ -1984,24 +2108,24 @@
         <v>53</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC12" s="10" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AD12" s="3" t="s">
         <v>60</v>
@@ -2021,18 +2145,18 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C13" s="7">
-        <v>2025090290</v>
+        <v>2025090282</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
-        <v>152</v>
+      <c r="F13" s="7">
+        <v>2890</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>42</v>
@@ -2046,7 +2170,7 @@
       <c r="O13" s="8"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="7" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>51</v>
@@ -2061,24 +2185,24 @@
         <v>53</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA13" s="7"/>
       <c r="AB13" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC13" s="9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AD13" s="7" t="s">
         <v>60</v>
@@ -2098,18 +2222,18 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C14" s="3">
-        <v>2025090294</v>
+        <v>2025090290</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3">
-        <v>5197</v>
+      <c r="F14" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>42</v>
@@ -2121,9 +2245,9 @@
       <c r="M14" s="4"/>
       <c r="N14" s="3"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="P14" s="10"/>
       <c r="Q14" s="3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>51</v>
@@ -2138,13 +2262,13 @@
         <v>53</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="X14" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3">
@@ -2154,8 +2278,8 @@
       <c r="AB14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC14" s="4" t="s">
-        <v>130</v>
+      <c r="AC14" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="AD14" s="3" t="s">
         <v>60</v>
@@ -2167,6 +2291,354 @@
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2025090294</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>5197</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T15" s="7">
+        <v>1</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2025090307</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3752</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC16" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2025090356</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2224</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2025090382</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>3752</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09021655
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$25</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="242">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-02  )</t>
   </si>
@@ -596,6 +596,45 @@
 換下：8185002487</t>
   </si>
   <si>
+    <t>14856114090101</t>
+  </si>
+  <si>
+    <t>新莊小胖店</t>
+  </si>
+  <si>
+    <t>2025-09-01 17:55:15</t>
+  </si>
+  <si>
+    <t>HL60</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET印票機L90</t>
+  </si>
+  <si>
+    <t>切刀卡紙，切紙不正常</t>
+  </si>
+  <si>
+    <t>門市反應LIFEET印票機L90無法正常裁切，已嘗試重啟設備+換裝新紙捲+簡易清潔仍異常..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04856</t>
+  </si>
+  <si>
+    <t>2025-09-01 17:57:33</t>
+  </si>
+  <si>
+    <t>2025-09-02 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 13:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 21:57:00</t>
+  </si>
+  <si>
+    <t>紙卷紙心變形無法列印 重裝紙卷</t>
+  </si>
+  <si>
     <t>E2224114090201</t>
   </si>
   <si>
@@ -636,6 +675,102 @@
   </si>
   <si>
     <t>2025-09-02 10:20:00</t>
+  </si>
+  <si>
+    <t>A171</t>
+  </si>
+  <si>
+    <t>淡水金龍店</t>
+  </si>
+  <si>
+    <t>新北市淡水區</t>
+  </si>
+  <si>
+    <t>THILF0A171</t>
+  </si>
+  <si>
+    <t>2025-09-02 11:30:21</t>
+  </si>
+  <si>
+    <t>2025-09-02 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 11:29:00</t>
+  </si>
+  <si>
+    <t>淡水屯山店</t>
+  </si>
+  <si>
+    <t>THILF04511</t>
+  </si>
+  <si>
+    <t>2025-09-02 12:47:16</t>
+  </si>
+  <si>
+    <t>2025-09-02 12:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 12:46:00</t>
+  </si>
+  <si>
+    <t>三芝芝蘭店</t>
+  </si>
+  <si>
+    <t>新北市三芝區</t>
+  </si>
+  <si>
+    <t>THILF02237</t>
+  </si>
+  <si>
+    <t>2025-09-02 13:23:36</t>
+  </si>
+  <si>
+    <t>2025-09-02 13:23:00</t>
+  </si>
+  <si>
+    <t>三芝天涯店</t>
+  </si>
+  <si>
+    <t>THILF04844</t>
+  </si>
+  <si>
+    <t>2025-09-02 14:38:15</t>
+  </si>
+  <si>
+    <t>2025-09-02 14:15:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 14:37:00</t>
+  </si>
+  <si>
+    <t>淡水櫻花店</t>
+  </si>
+  <si>
+    <t>THILF04739</t>
+  </si>
+  <si>
+    <t>2025-09-02 16:09:48</t>
+  </si>
+  <si>
+    <t>2025-09-02 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 16:09:00</t>
+  </si>
+  <si>
+    <t>淡水小坪頂</t>
+  </si>
+  <si>
+    <t>THILF05101</t>
+  </si>
+  <si>
+    <t>2025-09-02 16:44:14</t>
+  </si>
+  <si>
+    <t>2025-09-02 16:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 16:43:00</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1184,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK18"/>
+  <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC15" sqref="AC15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2476,7 +2611,7 @@
         <v>38</v>
       </c>
       <c r="C17" s="7">
-        <v>2025090356</v>
+        <v>2025090314</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>183</v>
@@ -2485,46 +2620,46 @@
         <v>40</v>
       </c>
       <c r="F17" s="7">
-        <v>2224</v>
+        <v>4856</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>184</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>185</v>
       </c>
       <c r="J17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="M17" s="8" t="s">
-        <v>47</v>
+        <v>187</v>
       </c>
       <c r="N17" s="7">
-        <v>2306</v>
+        <v>6001</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="T17" s="7">
         <v>1</v>
@@ -2533,16 +2668,16 @@
         <v>53</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="W17" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="X17" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Z17" s="7">
         <v>0.5</v>
@@ -2552,7 +2687,7 @@
         <v>58</v>
       </c>
       <c r="AC17" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AD17" s="7"/>
       <c r="AE17" s="7"/>
@@ -2570,32 +2705,52 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3">
-        <v>2025090382</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+        <v>2025090356</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F18" s="3">
-        <v>3752</v>
+        <v>2224</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
+      <c r="I18" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="3">
+        <v>2306</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>201</v>
+      </c>
       <c r="Q18" s="3" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>51</v>
@@ -2610,28 +2765,28 @@
         <v>53</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y18" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="Z18" s="3">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC18" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD18" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC18" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
@@ -2639,6 +2794,545 @@
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2025090382</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
+        <v>3752</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2025090406</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC20" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2025090413</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7">
+        <v>4511</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2025090417</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>2237</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC22" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2025090428</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <v>4844</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
+      <c r="AK23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2025090460</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>4739</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC24" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2025090467</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7">
+        <v>5101</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC25" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09031429
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$26</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="242">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-02  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="248">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-03  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -771,6 +771,24 @@
   </si>
   <si>
     <t>2025-09-02 16:43:00</t>
+  </si>
+  <si>
+    <t>淡水英才店</t>
+  </si>
+  <si>
+    <t>THILF04658</t>
+  </si>
+  <si>
+    <t>2025-09-03 12:48:12</t>
+  </si>
+  <si>
+    <t>2025-09-03 12:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-03 12:47:00</t>
+  </si>
+  <si>
+    <t>PMQ3+TVV</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1202,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK25"/>
+  <dimension ref="A1:AK26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3287,7 +3305,7 @@
       <c r="M25" s="8"/>
       <c r="N25" s="7"/>
       <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
+      <c r="P25" s="9"/>
       <c r="Q25" s="7" t="s">
         <v>238</v>
       </c>
@@ -3320,7 +3338,7 @@
       <c r="AB25" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC25" s="8" t="s">
+      <c r="AC25" s="9" t="s">
         <v>141</v>
       </c>
       <c r="AD25" s="7" t="s">
@@ -3333,6 +3351,83 @@
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
       <c r="AK25" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2025090599</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>4658</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC26" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09031537
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$27</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="253">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-03  )</t>
   </si>
@@ -789,6 +789,21 @@
   </si>
   <si>
     <t>PMQ3+TVV</t>
+  </si>
+  <si>
+    <t>淡水後洲店</t>
+  </si>
+  <si>
+    <t>THILF04298</t>
+  </si>
+  <si>
+    <t>2025-09-03 15:31:31</t>
+  </si>
+  <si>
+    <t>2025-09-03 15:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-03 15:30:00</t>
   </si>
 </sst>
 </file>
@@ -1202,10 +1217,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AK27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC23" sqref="AC23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3382,7 +3397,7 @@
       <c r="M26" s="4"/>
       <c r="N26" s="3"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="3" t="s">
         <v>243</v>
       </c>
@@ -3415,7 +3430,7 @@
       <c r="AB26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC26" s="4" t="s">
+      <c r="AC26" s="10" t="s">
         <v>247</v>
       </c>
       <c r="AD26" s="3" t="s">
@@ -3428,6 +3443,83 @@
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2025090650</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <v>4298</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC27" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7"/>
+      <c r="AK27" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09041655
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$37</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="253">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-03  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="320">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-04  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -773,6 +773,41 @@
     <t>2025-09-02 16:43:00</t>
   </si>
   <si>
+    <t>14145114090301</t>
+  </si>
+  <si>
+    <t>板橋僑興店</t>
+  </si>
+  <si>
+    <t>2025-09-03 10:51:42</t>
+  </si>
+  <si>
+    <t>星期三</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控異常鼠標會飄移到左上角且會亂點導致輸入顯示鼠標跳掉，已協助門市觸控校正重啟仍已異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04145</t>
+  </si>
+  <si>
+    <t>2025-09-03 10:53:36</t>
+  </si>
+  <si>
+    <t>2025-09-04 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 13:35:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:53:00</t>
+  </si>
+  <si>
+    <t>更換TCx800主機（硬碟無更換）
+換上：8185002961
+換下：8185002316</t>
+  </si>
+  <si>
     <t>淡水英才店</t>
   </si>
   <si>
@@ -804,6 +839,182 @@
   </si>
   <si>
     <t>2025-09-03 15:30:00</t>
+  </si>
+  <si>
+    <t>淡水國家店</t>
+  </si>
+  <si>
+    <t>THILF04788</t>
+  </si>
+  <si>
+    <t>2025-09-03 16:04:49</t>
+  </si>
+  <si>
+    <t>2025-09-03 15:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-03 16:03:00</t>
+  </si>
+  <si>
+    <t>13818114090401</t>
+  </si>
+  <si>
+    <t>板橋漢江店</t>
+  </si>
+  <si>
+    <t>2025-09-04 10:00:23</t>
+  </si>
+  <si>
+    <t>星期四</t>
+  </si>
+  <si>
+    <t>TM1(BSC10II)門市09/02反應稍早13點10分左右於TM1操作清帳後，入帳日已D+1，但未印出帳條，發票機燈號正常，TM未出現異常訊息，門市發票機為二代(BSC10II)，未操作任何基本排除後第一筆交易確認可正常印出發票，經hipos查看Eventlog無異常，收據檔內有此清帳帳條，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。今門市來電告知昨天又有交易未印出發票...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03818</t>
+  </si>
+  <si>
+    <t>2025-09-04 10:02:59</t>
+  </si>
+  <si>
+    <t>2025-09-04 15:45:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 16:12:00</t>
+  </si>
+  <si>
+    <t>2025-09-05 14:03:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上：8155006323
+換下：8155004152</t>
+  </si>
+  <si>
+    <t>14025114090402</t>
+  </si>
+  <si>
+    <t>新莊祐信店</t>
+  </si>
+  <si>
+    <t>2025-09-04 10:18:49</t>
+  </si>
+  <si>
+    <t>HL24</t>
+  </si>
+  <si>
+    <t>HL-SC主機</t>
+  </si>
+  <si>
+    <t>檔案損毀(更換硬碟)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025/9/4 (週四) 上午 10:18 總公司玫君MAIL:SC(SHUTTLE6S)4025新莊祐信店發生操作訂貨到一半會自動關閉，經檢視發現SC第一顆硬碟有異常，請到店更換SC第一顆硬碟不要備份還原， 請協助派工，並啟動緊急叫修...須請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳關到09/03，與通訊嘉芳確認都有收到
+</t>
+  </si>
+  <si>
+    <t>THILF04025</t>
+  </si>
+  <si>
+    <t>2025-09-04 10:27:47</t>
+  </si>
+  <si>
+    <t>2025-09-04 13:36:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 16:27:00</t>
+  </si>
+  <si>
+    <t>更換SC第一顆硬碟不備份還原，並告知更換許小姐硬碟注意事項
+HiPOS  最新版本= S0807.54.0   ARC.DEF = ARC4.815u
+SC = 20250805
+SC_Slave = 20250805</t>
+  </si>
+  <si>
+    <t>北縣板龍店</t>
+  </si>
+  <si>
+    <t>THILF02403</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:07:48</t>
+  </si>
+  <si>
+    <t>2025-09-04 13:45:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:05:00</t>
+  </si>
+  <si>
+    <t>D609</t>
+  </si>
+  <si>
+    <t>板橋大興店</t>
+  </si>
+  <si>
+    <t>THILF0D609</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:22:59</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:23:00</t>
+  </si>
+  <si>
+    <t>北縣板億店</t>
+  </si>
+  <si>
+    <t>THILF02422</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:41:28</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:26:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:40:00</t>
+  </si>
+  <si>
+    <t>板橋合安店</t>
+  </si>
+  <si>
+    <t>THILF04422</t>
+  </si>
+  <si>
+    <t>2025-09-04 15:08:41</t>
+  </si>
+  <si>
+    <t>2025-09-04 14:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 15:08:00</t>
+  </si>
+  <si>
+    <t>D161</t>
+  </si>
+  <si>
+    <t>北縣僑中三店</t>
+  </si>
+  <si>
+    <t>THILF0D161</t>
+  </si>
+  <si>
+    <t>2025-09-04 15:40:47</t>
+  </si>
+  <si>
+    <t>2025-09-04 15:15:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 15:35:00</t>
+  </si>
+  <si>
+    <t>2025-09-04 16:15:31</t>
   </si>
 </sst>
 </file>
@@ -1217,10 +1428,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK27"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3374,38 +3585,58 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3">
-        <v>2025090599</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+        <v>2025090555</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F26" s="3">
-        <v>4658</v>
+        <v>4145</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N26" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>246</v>
+      </c>
       <c r="Q26" s="3" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T26" s="3">
         <v>1</v>
@@ -3414,28 +3645,28 @@
         <v>53</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y26" s="3"/>
+        <v>250</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="Z26" s="3">
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC26" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="AD26" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
@@ -3454,15 +3685,15 @@
         <v>135</v>
       </c>
       <c r="C27" s="7">
-        <v>2025090650</v>
+        <v>2025090599</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7">
-        <v>4298</v>
+        <v>4658</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>212</v>
@@ -3474,9 +3705,9 @@
       <c r="M27" s="8"/>
       <c r="N27" s="7"/>
       <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
+      <c r="P27" s="9"/>
       <c r="Q27" s="7" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>51</v>
@@ -3491,24 +3722,24 @@
         <v>53</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="X27" s="7" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="Y27" s="7"/>
       <c r="Z27" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA27" s="7"/>
       <c r="AB27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC27" s="8" t="s">
-        <v>141</v>
+      <c r="AC27" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>60</v>
@@ -3522,6 +3753,816 @@
       <c r="AK27" s="7" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2025090650</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>4298</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2025090664</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
+        <v>4788</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T29" s="7">
+        <v>1</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
+      <c r="AJ29" s="7"/>
+      <c r="AK29" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2025090712</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="3">
+        <v>3818</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P30" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="Y30" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC30" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="7">
+        <v>2025090719</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" s="7">
+        <v>4025</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="N31" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T31" s="7">
+        <v>1</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="W31" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z31" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2025090785</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>2403</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T32" s="3">
+        <v>1</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC32" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2025090797</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2025090801</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>2422</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T34" s="3">
+        <v>1</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC34" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2025090805</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7">
+        <v>4422</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T35" s="7">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC35" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2025090814</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T36" s="3">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC36" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2025090821</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7">
+        <v>3818</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T37" s="7">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD37" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK37" s="7"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Auto commit - 09051246
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$38</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="320">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-04  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="329">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-05  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1015,6 +1015,34 @@
   </si>
   <si>
     <t>2025-09-04 16:15:31</t>
+  </si>
+  <si>
+    <t>14145114090401</t>
+  </si>
+  <si>
+    <t>2025-09-04 17:09:00</t>
+  </si>
+  <si>
+    <t>客顯示器畫面不正常</t>
+  </si>
+  <si>
+    <t>門市告知今日工程師到店協助更換TM2主機(TCX800)後客顯就黑畫面，門市表示查看客顯畫面線路未插，將線路插上後客顯畫面也呈現收銀的畫面，客服開啟觸控校正程式後門市告知兩個畫面都跳成客顯畫面，點選螢幕對應也無反應，協助重啟TM仍異常，VNC查看無出現客顯畫面僅有收銀畫面...請台芝到店協助
+※案14145114090301，台芝回覆:09/04 13:35 更換TCx800主機</t>
+  </si>
+  <si>
+    <t>2025-09-04 17:28:52</t>
+  </si>
+  <si>
+    <t>2025-09-05 11:08:00</t>
+  </si>
+  <si>
+    <t>2025-09-05 11:34:00</t>
+  </si>
+  <si>
+    <t>2025-09-05 21:28:00</t>
+  </si>
+  <si>
+    <t>線路重插後測試正常</t>
   </si>
 </sst>
 </file>
@@ -1428,10 +1456,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK37"/>
+  <dimension ref="A1:AK38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="AC35" sqref="AC35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4515,7 +4543,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="7"/>
       <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="P37" s="9"/>
       <c r="Q37" s="7" t="s">
         <v>274</v>
       </c>
@@ -4548,7 +4576,7 @@
       <c r="AB37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC37" s="8" t="s">
+      <c r="AC37" s="9" t="s">
         <v>141</v>
       </c>
       <c r="AD37" s="7" t="s">
@@ -4563,6 +4591,103 @@
         <v>60</v>
       </c>
       <c r="AK37" s="7"/>
+    </row>
+    <row r="38" spans="1:37">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2025090857</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="3">
+        <v>4145</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N38" s="3">
+        <v>2302</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T38" s="3">
+        <v>1</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="Y38" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC38" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+      <c r="AG38" s="3"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3"/>
+      <c r="AK38" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Auto commit - 09051800
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$39</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="342">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-05  )</t>
   </si>
@@ -1043,6 +1043,47 @@
   </si>
   <si>
     <t>線路重插後測試正常</t>
+  </si>
+  <si>
+    <t>E4698114090501</t>
+  </si>
+  <si>
+    <t>三重頂崁店</t>
+  </si>
+  <si>
+    <t>2025-09-05 10:00:06</t>
+  </si>
+  <si>
+    <t>HL25</t>
+  </si>
+  <si>
+    <t>HL-SC螢幕</t>
+  </si>
+  <si>
+    <t>螢幕畫面閃爍頻繁或無畫面</t>
+  </si>
+  <si>
+    <t>門市反應sc螢幕(LCD)會閃爍且螢幕會模糊看不清楚，門市已有重新拔插後方線路仍異常....須請台芝到店協助(店長桌電腦螢幕惚亮惚暗.霧霧的)</t>
+  </si>
+  <si>
+    <t>THILF04698</t>
+  </si>
+  <si>
+    <t>2025-09-05 10:16:02</t>
+  </si>
+  <si>
+    <t>2025-09-05 16:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-05 16:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:16:00</t>
+  </si>
+  <si>
+    <t>更換螢幕
+換下8133000923
+換上8133003666</t>
   </si>
 </sst>
 </file>
@@ -1456,10 +1497,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK38"/>
+  <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC35" sqref="AC35"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4638,7 +4679,7 @@
       <c r="O38" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="P38" s="4" t="s">
+      <c r="P38" s="10" t="s">
         <v>323</v>
       </c>
       <c r="Q38" s="3" t="s">
@@ -4675,7 +4716,7 @@
       <c r="AB38" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC38" s="4" t="s">
+      <c r="AC38" s="10" t="s">
         <v>328</v>
       </c>
       <c r="AD38" s="3"/>
@@ -4686,6 +4727,103 @@
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2025090911</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="7">
+        <v>4698</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="N39" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O39" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="P39" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T39" s="7">
+        <v>1</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z39" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC39" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+      <c r="AK39" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09081708
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$52</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="342">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-05  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="440">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-08  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -743,6 +743,48 @@
     <t>2025-09-02 14:37:00</t>
   </si>
   <si>
+    <t>15080114090201</t>
+  </si>
+  <si>
+    <t>三芝楓愛林</t>
+  </si>
+  <si>
+    <t>2025-09-02 14:53:58</t>
+  </si>
+  <si>
+    <t>HL99</t>
+  </si>
+  <si>
+    <t>HL-測試會勘</t>
+  </si>
+  <si>
+    <t>會勘</t>
+  </si>
+  <si>
+    <t>2025/9/2 (週二) 下午 02:17 總公司文豪MAIL: 5080三芝楓愛林4G訊號改善工程2024/12/11完成後，4G已正常撥上線，但還是會一直出現4G (Priority 2) disconnected (WAN failed PING test) in SIM slot A。為釐清問題9/8 (一) 10：00將進行多方會勘(遠傳、碩泰、台芝、HILIFE)，謝謝。請協助派工台芝(需攜帶一台Peplink 20X)</t>
+  </si>
+  <si>
+    <t>THILF05080</t>
+  </si>
+  <si>
+    <t>2025-09-02 14:57:11</t>
+  </si>
+  <si>
+    <t>2025-09-08 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 10:55:00</t>
+  </si>
+  <si>
+    <t>2025-09-03 18:57:00</t>
+  </si>
+  <si>
+    <t>111小時58分鐘</t>
+  </si>
+  <si>
+    <t>原機版本更新至8.5版，目前測試結果非設備問題，SIN卡外蓋遺失</t>
+  </si>
+  <si>
     <t>淡水櫻花店</t>
   </si>
   <si>
@@ -1084,6 +1126,265 @@
     <t>更換螢幕
 換下8133000923
 換上8133003666</t>
+  </si>
+  <si>
+    <t>13818114090501</t>
+  </si>
+  <si>
+    <t>2025-09-05 12:30:49</t>
+  </si>
+  <si>
+    <t>門市反應tm1 ccd掃描器(HC76-TR)常常刷讀所有條碼無反應有亮燈有逼聲，門市已有操作故掃描器校正仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-05 12:34:44</t>
+  </si>
+  <si>
+    <t>2025-09-08 11:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:34:00</t>
+  </si>
+  <si>
+    <t>1D349114090501</t>
+  </si>
+  <si>
+    <t>D349</t>
+  </si>
+  <si>
+    <t>板橋成都店</t>
+  </si>
+  <si>
+    <t>2025-09-05 13:30:41</t>
+  </si>
+  <si>
+    <t>門市反應TM1CC掃瞄槍(HC76-TR)有亮燈逼聲，但刷讀商品無反應，已有執行校正後仍異常，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D349</t>
+  </si>
+  <si>
+    <t>2025-09-05 13:32:31</t>
+  </si>
+  <si>
+    <t>2025-09-08 12:23:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 12:55:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 17:32:00</t>
+  </si>
+  <si>
+    <t>更換CCD掃槍
+換上：8119011523
+換下：8119012066</t>
+  </si>
+  <si>
+    <t>1D649114090601</t>
+  </si>
+  <si>
+    <t>D649</t>
+  </si>
+  <si>
+    <t>三重運動公園</t>
+  </si>
+  <si>
+    <t>2025-09-06 10:51:02</t>
+  </si>
+  <si>
+    <t>門市反應tm2(tcx800)觸控不良操作訂貨時左上方位置無法觸控，已協助操作螢幕校正仍異常，與門市確認螢幕無保護貼、文宣....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D649</t>
+  </si>
+  <si>
+    <t>2025-09-06 10:53:13</t>
+  </si>
+  <si>
+    <t>2025-09-08 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:28:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 13:00:00</t>
+  </si>
+  <si>
+    <t>更換主機，無更換硬碟
+換下8185000697
+換上8185000168</t>
+  </si>
+  <si>
+    <t>ED087114090601</t>
+  </si>
+  <si>
+    <t>D087</t>
+  </si>
+  <si>
+    <t>三重中興北</t>
+  </si>
+  <si>
+    <t>2025-09-06 12:09:03</t>
+  </si>
+  <si>
+    <t>門市反應LIFEET印票機L90無電源反應，已有按壓電源鍵、重新拔插線路仍異常...請台芝到店協助(票券機之電源無反應)</t>
+  </si>
+  <si>
+    <t>THILF0D087</t>
+  </si>
+  <si>
+    <t>2025-09-06 12:18:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:25:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:55:00</t>
+  </si>
+  <si>
+    <t>電源線脫落，插上後正常</t>
+  </si>
+  <si>
+    <t>林口大千苑店</t>
+  </si>
+  <si>
+    <t>新北市林口區</t>
+  </si>
+  <si>
+    <t>THILF04834</t>
+  </si>
+  <si>
+    <t>2025-09-08 09:57:21</t>
+  </si>
+  <si>
+    <t>2025-09-08 09:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 09:30:00</t>
+  </si>
+  <si>
+    <t>林口建林店</t>
+  </si>
+  <si>
+    <t>THILF04282</t>
+  </si>
+  <si>
+    <t>2025-09-08 10:06:16</t>
+  </si>
+  <si>
+    <t>林口捷韻店</t>
+  </si>
+  <si>
+    <t>THILF04715</t>
+  </si>
+  <si>
+    <t>2025-09-08 10:21:35</t>
+  </si>
+  <si>
+    <t>2025-09-08 10:30:00</t>
+  </si>
+  <si>
+    <t>林口建安店</t>
+  </si>
+  <si>
+    <t>THILF04326</t>
+  </si>
+  <si>
+    <t>2025-09-08 11:26:10</t>
+  </si>
+  <si>
+    <t>2025-09-08 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 11:30:00</t>
+  </si>
+  <si>
+    <t>15384114090801</t>
+  </si>
+  <si>
+    <t>板橋民生站</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:20:20</t>
+  </si>
+  <si>
+    <t>門市告知稍早TM1(TCX800)清帳時突然動到後，就無法再開機，已自行將線路重新拔插後仍異常，電源燈無亮燈，門市已確認線路無鬆脫、更換至白色插座仍異常...請台芝到店協助 已與門市確認09/08有交易帳條無印出PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)</t>
+  </si>
+  <si>
+    <t>THILF05384</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:24:17</t>
+  </si>
+  <si>
+    <t>2025-09-08 15:17:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 15:47:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 17:24:00</t>
+  </si>
+  <si>
+    <t>林口築夢店</t>
+  </si>
+  <si>
+    <t>THILF04483</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:26:35</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:30:00</t>
+  </si>
+  <si>
+    <t>林口老師店</t>
+  </si>
+  <si>
+    <t>THILF04514</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:54:58</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:00:00</t>
+  </si>
+  <si>
+    <t>15384114090802</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:51:37</t>
+  </si>
+  <si>
+    <t>當機</t>
+  </si>
+  <si>
+    <t>09/08 14:50總公司玫君來電啟動緊急叫修:門市告知稍早TM1(TCX800)清帳時突然動到後，就無法再開機，已自行將線路重新拔插後仍異常，電源燈無亮燈，門市已確認線路無鬆脫、更換至白色插座仍異常...請台芝到店協助 已與門市確認09/08有交易帳條無印出PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:52:36</t>
+  </si>
+  <si>
+    <t>2025-09-08 15:36:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 07:52:00</t>
+  </si>
+  <si>
+    <t>重新接電後正常開機，更換變壓器觀察
+1.開機後入帳日仍為2025/09/08
+2.登入收銀員顯示多日未清障
+3.清障後與騰雲確認帳務無異常</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1798,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK39"/>
+  <dimension ref="A1:AK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="AC49" sqref="AC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3500,32 +3801,52 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C24" s="3">
-        <v>2025090460</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+        <v>2025090433</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F24" s="3">
-        <v>4739</v>
+        <v>5080</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="N24" s="3">
+        <v>9902</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>238</v>
+      </c>
       <c r="Q24" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>51</v>
@@ -3540,28 +3861,30 @@
         <v>53</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="Y24" s="3"/>
+        <v>242</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="Z24" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="AA24" s="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>244</v>
+      </c>
       <c r="AB24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC24" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD24" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
@@ -3580,15 +3903,15 @@
         <v>135</v>
       </c>
       <c r="C25" s="7">
-        <v>2025090467</v>
+        <v>2025090460</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7">
-        <v>5101</v>
+        <v>4739</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>212</v>
@@ -3602,7 +3925,7 @@
       <c r="O25" s="8"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="7" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>51</v>
@@ -3617,17 +3940,17 @@
         <v>53</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="X25" s="7" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="Y25" s="7"/>
       <c r="Z25" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA25" s="7"/>
       <c r="AB25" s="7" t="s">
@@ -3654,58 +3977,38 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="C26" s="3">
-        <v>2025090555</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>2025090467</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="3">
-        <v>4145</v>
+        <v>5101</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N26" s="3">
-        <v>2307</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="P26" s="10" t="s">
-        <v>246</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="3" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T26" s="3">
         <v>1</v>
@@ -3714,28 +4017,28 @@
         <v>53</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="Y26" s="3" t="s">
-        <v>251</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="Y26" s="3"/>
       <c r="Z26" s="3">
-        <v>1.6</v>
+        <v>0.4</v>
       </c>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC26" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="AD26" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
@@ -3751,38 +4054,58 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C27" s="7">
-        <v>2025090599</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+        <v>2025090555</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F27" s="7">
-        <v>4658</v>
+        <v>4145</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N27" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="Q27" s="7" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T27" s="7">
         <v>1</v>
@@ -3791,28 +4114,28 @@
         <v>53</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="X27" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y27" s="7"/>
+        <v>264</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="Z27" s="7">
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
       <c r="AA27" s="7"/>
       <c r="AB27" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC27" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="AD27" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="AD27" s="7"/>
       <c r="AE27" s="7"/>
       <c r="AF27" s="7"/>
       <c r="AG27" s="7"/>
@@ -3831,15 +4154,15 @@
         <v>135</v>
       </c>
       <c r="C28" s="3">
-        <v>2025090650</v>
+        <v>2025090599</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3">
-        <v>4298</v>
+        <v>4658</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>212</v>
@@ -3853,7 +4176,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="3" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>51</v>
@@ -3868,24 +4191,24 @@
         <v>53</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA28" s="3"/>
       <c r="AB28" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC28" s="10" t="s">
-        <v>141</v>
+        <v>272</v>
       </c>
       <c r="AD28" s="3" t="s">
         <v>60</v>
@@ -3908,15 +4231,15 @@
         <v>135</v>
       </c>
       <c r="C29" s="7">
-        <v>2025090664</v>
+        <v>2025090650</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
-        <v>4788</v>
+        <v>4298</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>212</v>
@@ -3930,7 +4253,7 @@
       <c r="O29" s="8"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="7" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>51</v>
@@ -3945,17 +4268,17 @@
         <v>53</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7" t="s">
@@ -3982,58 +4305,38 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="C30" s="3">
-        <v>2025090712</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>2025090664</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="3">
-        <v>3818</v>
+        <v>4788</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="P30" s="10" t="s">
-        <v>273</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="10"/>
       <c r="Q30" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T30" s="3">
         <v>1</v>
@@ -4042,28 +4345,28 @@
         <v>53</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="Y30" s="3" t="s">
-        <v>278</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="Y30" s="3"/>
       <c r="Z30" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA30" s="3"/>
       <c r="AB30" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC30" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="AD30" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="AD30" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
@@ -4082,55 +4385,55 @@
         <v>38</v>
       </c>
       <c r="C31" s="7">
-        <v>2025090719</v>
+        <v>2025090712</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="F31" s="7">
-        <v>4025</v>
+        <v>3818</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>116</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>283</v>
+        <v>66</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="N31" s="7">
-        <v>2405</v>
+        <v>67</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>285</v>
+        <v>69</v>
       </c>
       <c r="P31" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="T31" s="7">
         <v>1</v>
@@ -4139,26 +4442,26 @@
         <v>53</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="W31" s="7" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
       <c r="X31" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="Z31" s="7">
-        <v>1.6</v>
+        <v>0.5</v>
       </c>
       <c r="AA31" s="7"/>
       <c r="AB31" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC31" s="9" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AD31" s="7"/>
       <c r="AE31" s="7"/>
@@ -4176,38 +4479,58 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3">
-        <v>2025090785</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+        <v>2025090719</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="F32" s="3">
-        <v>2403</v>
+        <v>4025</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="10"/>
+        <v>80</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P32" s="10" t="s">
+        <v>300</v>
+      </c>
       <c r="Q32" s="3" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="T32" s="3">
         <v>1</v>
@@ -4216,28 +4539,28 @@
         <v>53</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="Y32" s="3"/>
+        <v>303</v>
+      </c>
+      <c r="Y32" s="3" t="s">
+        <v>304</v>
+      </c>
       <c r="Z32" s="3">
-        <v>0.3</v>
+        <v>1.6</v>
       </c>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC32" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD32" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
@@ -4256,15 +4579,15 @@
         <v>135</v>
       </c>
       <c r="C33" s="7">
-        <v>2025090797</v>
+        <v>2025090785</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="7" t="s">
-        <v>297</v>
+      <c r="F33" s="7">
+        <v>2403</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>63</v>
@@ -4278,7 +4601,7 @@
       <c r="O33" s="8"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="7" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>51</v>
@@ -4293,17 +4616,17 @@
         <v>53</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="W33" s="7" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="X33" s="7" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="AA33" s="7"/>
       <c r="AB33" s="7" t="s">
@@ -4333,15 +4656,15 @@
         <v>135</v>
       </c>
       <c r="C34" s="3">
-        <v>2025090801</v>
+        <v>2025090797</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3">
-        <v>2422</v>
+      <c r="F34" s="3" t="s">
+        <v>311</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>63</v>
@@ -4355,7 +4678,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="3" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>51</v>
@@ -4370,13 +4693,13 @@
         <v>53</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3">
@@ -4410,15 +4733,15 @@
         <v>135</v>
       </c>
       <c r="C35" s="7">
-        <v>2025090805</v>
+        <v>2025090801</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <v>4422</v>
+        <v>2422</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>63</v>
@@ -4432,7 +4755,7 @@
       <c r="O35" s="8"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="7" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>51</v>
@@ -4447,17 +4770,17 @@
         <v>53</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AA35" s="7"/>
       <c r="AB35" s="7" t="s">
@@ -4487,15 +4810,15 @@
         <v>135</v>
       </c>
       <c r="C36" s="3">
-        <v>2025090814</v>
+        <v>2025090805</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
-        <v>313</v>
+      <c r="F36" s="3">
+        <v>4422</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>63</v>
@@ -4509,7 +4832,7 @@
       <c r="O36" s="4"/>
       <c r="P36" s="10"/>
       <c r="Q36" s="3" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>51</v>
@@ -4524,13 +4847,13 @@
         <v>53</v>
       </c>
       <c r="V36" s="3" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="X36" s="3" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3">
@@ -4564,15 +4887,15 @@
         <v>135</v>
       </c>
       <c r="C37" s="7">
-        <v>2025090821</v>
+        <v>2025090814</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="7">
-        <v>3818</v>
+      <c r="F37" s="7" t="s">
+        <v>327</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>270</v>
+        <v>328</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>63</v>
@@ -4586,7 +4909,7 @@
       <c r="O37" s="8"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="7" t="s">
-        <v>274</v>
+        <v>329</v>
       </c>
       <c r="R37" s="7" t="s">
         <v>51</v>
@@ -4601,17 +4924,17 @@
         <v>53</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="W37" s="7" t="s">
-        <v>276</v>
+        <v>331</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>277</v>
+        <v>332</v>
       </c>
       <c r="Y37" s="7"/>
       <c r="Z37" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA37" s="7"/>
       <c r="AB37" s="7" t="s">
@@ -4628,62 +4951,42 @@
       <c r="AG37" s="7"/>
       <c r="AH37" s="7"/>
       <c r="AI37" s="7"/>
-      <c r="AJ37" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="38" spans="1:37">
       <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="C38" s="3">
-        <v>2025090857</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>2025090821</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="3">
-        <v>4145</v>
+        <v>3818</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>243</v>
+        <v>284</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N38" s="3">
-        <v>2302</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>323</v>
-      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="10"/>
       <c r="Q38" s="3" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="R38" s="3" t="s">
         <v>51</v>
@@ -4698,37 +5001,37 @@
         <v>53</v>
       </c>
       <c r="V38" s="3" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
       <c r="X38" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="Y38" s="3" t="s">
-        <v>327</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="Y38" s="3"/>
       <c r="Z38" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC38" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="AD38" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="AD38" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE38" s="3"/>
       <c r="AF38" s="3"/>
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
-      <c r="AJ38" s="3"/>
-      <c r="AK38" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK38" s="3"/>
     </row>
     <row r="39" spans="1:37">
       <c r="A39" s="7">
@@ -4738,55 +5041,55 @@
         <v>38</v>
       </c>
       <c r="C39" s="7">
-        <v>2025090911</v>
+        <v>2025090857</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F39" s="7">
-        <v>4698</v>
+        <v>4145</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>330</v>
+        <v>257</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>44</v>
+        <v>286</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>332</v>
+        <v>46</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>333</v>
+        <v>47</v>
       </c>
       <c r="N39" s="7">
-        <v>2501</v>
+        <v>2302</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="P39" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
+      </c>
+      <c r="P39" s="9" t="s">
+        <v>337</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>336</v>
+        <v>261</v>
       </c>
       <c r="R39" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S39" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="T39" s="7">
         <v>1</v>
@@ -4795,26 +5098,26 @@
         <v>53</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="W39" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="X39" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="Y39" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Z39" s="7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA39" s="7"/>
       <c r="AB39" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC39" s="8" t="s">
-        <v>341</v>
+      <c r="AC39" s="9" t="s">
+        <v>342</v>
       </c>
       <c r="AD39" s="7"/>
       <c r="AE39" s="7"/>
@@ -4824,6 +5127,1149 @@
       <c r="AI39" s="7"/>
       <c r="AJ39" s="7"/>
       <c r="AK39" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2025090911</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="3">
+        <v>4698</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="N40" s="3">
+        <v>2501</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T40" s="3">
+        <v>1</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y40" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="Z40" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC40" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2025090957</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="7">
+        <v>3818</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P41" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="R41" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T41" s="7">
+        <v>1</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="X41" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC41" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD41" s="7"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+      <c r="AK41" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2025090963</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T42" s="3">
+        <v>1</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC42" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
+      <c r="AG42" s="3"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
+      <c r="AJ42" s="3"/>
+      <c r="AK42" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2025091038</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N43" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P43" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="R43" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T43" s="7">
+        <v>1</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z43" s="7">
+        <v>1.1</v>
+      </c>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC43" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="AD43" s="7"/>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2025091040</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="N44" s="3">
+        <v>6004</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="P44" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T44" s="3">
+        <v>1</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC44" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="AD44" s="3"/>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+      <c r="AG44" s="3"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
+      <c r="AJ44" s="3"/>
+      <c r="AK44" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2025091069</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7">
+        <v>4834</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="R45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T45" s="7">
+        <v>1</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="W45" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="X45" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC45" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD45" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE45" s="7"/>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="7"/>
+      <c r="AK45" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2025091070</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3">
+        <v>4282</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T46" s="3">
+        <v>1</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC46" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
+      <c r="AG46" s="3"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="3"/>
+      <c r="AJ46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK46" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="7">
+        <v>2025091076</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7">
+        <v>4715</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T47" s="7">
+        <v>1</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC47" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="7"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="7"/>
+      <c r="AK47" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2025091095</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3">
+        <v>4326</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T48" s="3">
+        <v>1</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC48" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3"/>
+      <c r="AK48" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2025091105</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="7">
+        <v>5384</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N49" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O49" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="P49" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T49" s="7">
+        <v>1</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="W49" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="X49" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y49" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="Z49" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC49" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD49" s="7"/>
+      <c r="AE49" s="7"/>
+      <c r="AF49" s="7"/>
+      <c r="AG49" s="7"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7"/>
+      <c r="AK49" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2025091106</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3">
+        <v>4483</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T50" s="3">
+        <v>1</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="3"/>
+      <c r="AG50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="7">
+        <v>2025091113</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7">
+        <v>4514</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T51" s="7">
+        <v>1</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC51" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD51" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2025091130</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F52" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N52" s="3">
+        <v>2301</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T52" s="3">
+        <v>1</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="Y52" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="Z52" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC52" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD52" s="3"/>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+      <c r="AH52" s="3"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="3"/>
+      <c r="AK52" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09101044
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$63</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="440">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-08  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="525">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-10  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1276,6 +1276,47 @@
     <t>2025-09-08 10:06:16</t>
   </si>
   <si>
+    <t>13751114090802</t>
+  </si>
+  <si>
+    <t>淡水真理大</t>
+  </si>
+  <si>
+    <t>2025-09-08 09:59:49</t>
+  </si>
+  <si>
+    <t>HL34</t>
+  </si>
+  <si>
+    <t>HL-HUB</t>
+  </si>
+  <si>
+    <t>不能連線</t>
+  </si>
+  <si>
+    <t>HUB(DGS1210-28)-門市今日暫歇回來開PORT，客服PING91有通但無法連線91HUB，無法操作開PORT，後續請門市手動重啟HUB後PORT已自動打開，但仍無法連91HUB..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03751</t>
+  </si>
+  <si>
+    <t>2025-09-08 10:11:05</t>
+  </si>
+  <si>
+    <t>2025-09-09 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 13:32:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 14:11:00</t>
+  </si>
+  <si>
+    <t>更換HUB
+換下8107004306
+換上8107005200</t>
+  </si>
+  <si>
     <t>林口捷韻店</t>
   </si>
   <si>
@@ -1288,6 +1329,38 @@
     <t>2025-09-08 10:30:00</t>
   </si>
   <si>
+    <t>13751114090803</t>
+  </si>
+  <si>
+    <t>2025-09-08 11:12:50</t>
+  </si>
+  <si>
+    <t>當機/自動開關機</t>
+  </si>
+  <si>
+    <t>9/8 11:00 總公司明翰告知一般叫修：門市為暫歇門市，今日回店欲操作訂貨，發現SC(SHUTTLE5S)黑屏，已確認主機電源燈有亮藍燈，門市有將插頭拔掉放電5分鐘後插回重啟仍異常，ping1不通無法vnc...需請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認暫歇前帳務做到06/13，與通訊功評確認有收到的銷售
+***店長告知9/8 17:30前，9/9 09:00-17點前皆在門市，請工程師到店前先電話聯繫
+店長手機0908828877</t>
+  </si>
+  <si>
+    <t>2025-09-08 11:14:12</t>
+  </si>
+  <si>
+    <t>2025-09-09 17:59:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 15:14:00</t>
+  </si>
+  <si>
+    <t>2小時45分鐘</t>
+  </si>
+  <si>
+    <t>原機5S  VGA頭損壞需更換主機，更換成6S，比且需做第一顆和第二顆硬碟不備份還原
+更換主機
+換下8114003057
+換上8114004019</t>
+  </si>
+  <si>
     <t>林口建安店</t>
   </si>
   <si>
@@ -1343,6 +1416,60 @@
   </si>
   <si>
     <t>2025-09-08 13:30:00</t>
+  </si>
+  <si>
+    <t>13243114090801</t>
+  </si>
+  <si>
+    <t>北縣醒吾店</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:23:16</t>
+  </si>
+  <si>
+    <t>HL27</t>
+  </si>
+  <si>
+    <t>HL-雷射印表機</t>
+  </si>
+  <si>
+    <t>無法進紙、印表機無反應</t>
+  </si>
+  <si>
+    <t>門市反應sc雷射印表機(M6600NW)無法列印資料，查看門市印表機設定狀態顯示離線，與門市確認雷射印表機畫面正常有開機重啟後仍異常，協助移除後重新新增裝置但都查無設備....須請台芝到店協助
+**學校門市尚未正式營業今明兩天門市只會待到13點，後天才會待到下午，請工程師到店前可先連絡店長確認</t>
+  </si>
+  <si>
+    <t>THILF03243</t>
+  </si>
+  <si>
+    <t>2025-09-08 13:27:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 15:33:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 16:03:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 17:27:00</t>
+  </si>
+  <si>
+    <t>配合門市營業時間，已跟店長約修09/10 0930</t>
+  </si>
+  <si>
+    <t>2025-09-10 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 09:50:00</t>
+  </si>
+  <si>
+    <t>16小時23分鐘</t>
+  </si>
+  <si>
+    <t>更換印表機
+換上8103002250
+換下8103001960</t>
   </si>
   <si>
     <t>林口老師店</t>
@@ -1385,6 +1512,157 @@
 1.開機後入帳日仍為2025/09/08
 2.登入收銀員顯示多日未清障
 3.清障後與騰雲確認帳務無異常</t>
+  </si>
+  <si>
+    <t>14326114090801</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:14:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市於9/6反應TM1清帳未印出帳條及退瓶，只印出一小截空白，與門市確認當下發票機燈號正常，TM未出現異常訊息，未操作任何基本排除後續交易發票出紙正常，發票機為二代（BSC10II）。hipos回覆:查看退瓶有入帳，收據檔內有此張退瓶收據、清帳帳條，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。門市今日告知tm1帳條仍僅印出一小截空白...請台芝到店協助
+</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:18:23</t>
+  </si>
+  <si>
+    <t>2025-09-09 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 20:18:00</t>
+  </si>
+  <si>
+    <t>更壞發票機
+換上8155004446
+換下8155004375</t>
+  </si>
+  <si>
+    <t>14326114090802</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:14:44</t>
+  </si>
+  <si>
+    <t>門市於9/6反應TM2清帳未印出帳條及退瓶，只印出一小截空白，與門市確認當下發票機燈號正常，TM未出現異常訊息，未操作任何基本排除後續交易發票出紙正常，發票機為二代（BSC10II）。hipos回覆:查看退瓶有入帳，收據檔內有此張退瓶收據、清帳帳條，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。門市今日告知今日tm2有正常出帳條但仍須請工程師協助到店查看...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:19:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 20:19:00</t>
+  </si>
+  <si>
+    <t>更壞發票機
+換上8155005469
+換下8155004374</t>
+  </si>
+  <si>
+    <t>15352114090801</t>
+  </si>
+  <si>
+    <t>三重重陽店</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:20:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM2發票機（BSC10II）-門市告知前天TM2清帳印出的退瓶是空白的，印出的帳條正常，與門市確認當下發票機燈號正常，TM未出現異常訊息，未操作任何基本排除後續交易發票出紙正常，發票機為二代（BSC10II），因收據無法補印。總公司規定門市應落實張貼交回，遺失此憑證將視為短匯(會扣錢)經HIPOS查看Eventlog無異常，收據檔內有此清帳帳條，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。與門市確認此狀況頻繁發生，且發票明細等都會有此狀況....須請台芝到店協助 </t>
+  </si>
+  <si>
+    <t>THILF05352</t>
+  </si>
+  <si>
+    <t>2025-09-08 16:23:30</t>
+  </si>
+  <si>
+    <t>2025-09-09 18:51:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 19:21:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 20:23:00</t>
+  </si>
+  <si>
+    <t>現場測試正常
+更換發票機
+換下8155004455
+換上8155004154</t>
+  </si>
+  <si>
+    <t>15291114090902</t>
+  </si>
+  <si>
+    <t>新莊國家置地</t>
+  </si>
+  <si>
+    <t>2025-09-09 10:47:50</t>
+  </si>
+  <si>
+    <t>SC(SHUTTLE6S)-門市反應TM主檔卡在9/8無法更新，查看SC主檔09/09正確，協助SC轉TM後10分鐘版本更新仍異常。到最高權限操作手動排除主檔無法更新後SC轉TM10分鐘後版本更新仍異常，總公司功評查看有出現SC.Service服務意外地終止。已經發生N次。之訊息，請派工到店更換SC第二顆硬碟不備份還原。...須請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳關到09/08，與通訊圭連確認都有收到</t>
+  </si>
+  <si>
+    <t>THILF05291</t>
+  </si>
+  <si>
+    <t>2025-09-09 10:52:08</t>
+  </si>
+  <si>
+    <t>2025-09-09 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 14:52:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">更換一二顆硬碟不備份還原，並告知吳小姐更換硬碟注意事項。
+SC = 20250805
+SC_Slave = 20250805
+</t>
+  </si>
+  <si>
+    <t>2025-09-09 18:02:29</t>
+  </si>
+  <si>
+    <t>2025-09-09 17:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-09 18:00:00</t>
+  </si>
+  <si>
+    <t>PMQ3+PEP安裝完成</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:01:35</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:10:00</t>
+  </si>
+  <si>
+    <t>北縣黎明店</t>
+  </si>
+  <si>
+    <t>新北市泰山區</t>
+  </si>
+  <si>
+    <t>THILF03137</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:30:11</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:30:00</t>
   </si>
 </sst>
 </file>
@@ -1798,10 +2076,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK52"/>
+  <dimension ref="A1:AK63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC49" sqref="AC49"/>
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5776,38 +6054,58 @@
         <v>45</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C47" s="7">
-        <v>2025091076</v>
-      </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
+        <v>2025091072</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F47" s="7">
-        <v>4715</v>
+        <v>3751</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="9"/>
+        <v>212</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="N47" s="7">
+        <v>3402</v>
+      </c>
+      <c r="O47" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="P47" s="9" t="s">
+        <v>410</v>
+      </c>
       <c r="Q47" s="7" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S47" s="7" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="T47" s="7">
         <v>1</v>
@@ -5816,28 +6114,28 @@
         <v>53</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="W47" s="7" t="s">
-        <v>241</v>
+        <v>413</v>
       </c>
       <c r="X47" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="Y47" s="7"/>
+        <v>414</v>
+      </c>
+      <c r="Y47" s="7" t="s">
+        <v>415</v>
+      </c>
       <c r="Z47" s="7">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="AA47" s="7"/>
       <c r="AB47" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC47" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD47" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>416</v>
+      </c>
+      <c r="AD47" s="7"/>
       <c r="AE47" s="7"/>
       <c r="AF47" s="7"/>
       <c r="AG47" s="7"/>
@@ -5856,15 +6154,15 @@
         <v>135</v>
       </c>
       <c r="C48" s="3">
-        <v>2025091095</v>
+        <v>2025091076</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3">
-        <v>4326</v>
+        <v>4715</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>396</v>
@@ -5878,7 +6176,7 @@
       <c r="O48" s="4"/>
       <c r="P48" s="10"/>
       <c r="Q48" s="3" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="R48" s="3" t="s">
         <v>51</v>
@@ -5893,13 +6191,13 @@
         <v>53</v>
       </c>
       <c r="V48" s="3" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="W48" s="3" t="s">
-        <v>411</v>
+        <v>241</v>
       </c>
       <c r="X48" s="3" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="Y48" s="3"/>
       <c r="Z48" s="3">
@@ -5933,55 +6231,55 @@
         <v>38</v>
       </c>
       <c r="C49" s="7">
-        <v>2025091105</v>
+        <v>2025091093</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F49" s="7">
-        <v>5384</v>
+        <v>3751</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>63</v>
+        <v>212</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="J49" s="7" t="s">
         <v>127</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>46</v>
+        <v>297</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>47</v>
+        <v>298</v>
       </c>
       <c r="N49" s="7">
-        <v>2306</v>
+        <v>2401</v>
       </c>
       <c r="O49" s="8" t="s">
-        <v>200</v>
+        <v>423</v>
       </c>
       <c r="P49" s="9" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="Q49" s="7" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="R49" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S49" s="7" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T49" s="7">
         <v>1</v>
@@ -5990,26 +6288,28 @@
         <v>53</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="W49" s="7" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="X49" s="7" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="Y49" s="7" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="Z49" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="AA49" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="AA49" s="7" t="s">
+        <v>428</v>
+      </c>
       <c r="AB49" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC49" s="9" t="s">
-        <v>134</v>
+        <v>429</v>
       </c>
       <c r="AD49" s="7"/>
       <c r="AE49" s="7"/>
@@ -6030,15 +6330,15 @@
         <v>135</v>
       </c>
       <c r="C50" s="3">
-        <v>2025091106</v>
+        <v>2025091095</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3">
-        <v>4483</v>
+        <v>4326</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>396</v>
@@ -6052,7 +6352,7 @@
       <c r="O50" s="4"/>
       <c r="P50" s="10"/>
       <c r="Q50" s="3" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
       <c r="R50" s="3" t="s">
         <v>51</v>
@@ -6067,13 +6367,13 @@
         <v>53</v>
       </c>
       <c r="V50" s="3" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="W50" s="3" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="X50" s="3" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="Y50" s="3"/>
       <c r="Z50" s="3">
@@ -6104,38 +6404,58 @@
         <v>49</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C51" s="7">
-        <v>2025091113</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
+        <v>2025091105</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F51" s="7">
-        <v>4514</v>
+        <v>5384</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N51" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O51" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="P51" s="9" t="s">
+        <v>438</v>
+      </c>
       <c r="Q51" s="7" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="R51" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S51" s="7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="T51" s="7">
         <v>1</v>
@@ -6144,15 +6464,17 @@
         <v>53</v>
       </c>
       <c r="V51" s="7" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="W51" s="7" t="s">
-        <v>426</v>
+        <v>441</v>
       </c>
       <c r="X51" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="Y51" s="7"/>
+        <v>442</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>443</v>
+      </c>
       <c r="Z51" s="7">
         <v>0.5</v>
       </c>
@@ -6161,11 +6483,9 @@
         <v>58</v>
       </c>
       <c r="AC51" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD51" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AD51" s="7"/>
       <c r="AE51" s="7"/>
       <c r="AF51" s="7"/>
       <c r="AG51" s="7"/>
@@ -6181,58 +6501,38 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="C52" s="3">
-        <v>2025091130</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>175</v>
-      </c>
+        <v>2025091106</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
       <c r="F52" s="3">
-        <v>5384</v>
+        <v>4483</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>414</v>
+        <v>444</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M52" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N52" s="3">
-        <v>2301</v>
-      </c>
-      <c r="O52" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="P52" s="4" t="s">
-        <v>434</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="10"/>
       <c r="Q52" s="3" t="s">
-        <v>417</v>
+        <v>445</v>
       </c>
       <c r="R52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="T52" s="3">
         <v>1</v>
@@ -6241,28 +6541,28 @@
         <v>53</v>
       </c>
       <c r="V52" s="3" t="s">
-        <v>435</v>
+        <v>446</v>
       </c>
       <c r="W52" s="3" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="X52" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="Y52" s="3" t="s">
-        <v>438</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="Y52" s="3"/>
       <c r="Z52" s="3">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="AA52" s="3"/>
       <c r="AB52" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC52" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="AD52" s="3"/>
+      <c r="AC52" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE52" s="3"/>
       <c r="AF52" s="3"/>
       <c r="AG52" s="3"/>
@@ -6270,6 +6570,997 @@
       <c r="AI52" s="3"/>
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="7">
+        <v>2025091107</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="7">
+        <v>3243</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="N53" s="7">
+        <v>2702</v>
+      </c>
+      <c r="O53" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="P53" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q53" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T53" s="7">
+        <v>1</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V53" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="W53" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="X53" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="Y53" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="Z53" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC53" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="AD53" s="7"/>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2025091107</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="3">
+        <v>3243</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="N54" s="3">
+        <v>2702</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="P54" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T54" s="3">
+        <v>2</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="X54" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="Z54" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC54" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="AD54" s="3"/>
+      <c r="AE54" s="3"/>
+      <c r="AF54" s="3"/>
+      <c r="AG54" s="3"/>
+      <c r="AH54" s="3"/>
+      <c r="AI54" s="3"/>
+      <c r="AJ54" s="3"/>
+      <c r="AK54" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="7">
+        <v>2025091113</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7">
+        <v>4514</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T55" s="7">
+        <v>1</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC55" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD55" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE55" s="7"/>
+      <c r="AF55" s="7"/>
+      <c r="AG55" s="7"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7"/>
+      <c r="AK55" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="3">
+        <v>2025091130</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F56" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N56" s="3">
+        <v>2301</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="P56" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q56" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S56" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T56" s="3">
+        <v>1</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="X56" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="Y56" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="Z56" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC56" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+      <c r="AK56" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="7">
+        <v>2025091249</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="7">
+        <v>4326</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M57" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O57" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P57" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T57" s="7">
+        <v>1</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V57" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="W57" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y57" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z57" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC57" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="AD57" s="7"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7"/>
+      <c r="AK57" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2025091251</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="3">
+        <v>4326</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P58" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T58" s="3">
+        <v>1</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V58" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="X58" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="Y58" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="Z58" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC58" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="AD58" s="3"/>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="3"/>
+      <c r="AG58" s="3"/>
+      <c r="AH58" s="3"/>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="3"/>
+      <c r="AK58" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="7">
+        <v>2025091253</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="7">
+        <v>5352</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M59" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N59" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O59" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P59" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q59" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T59" s="7">
+        <v>1</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V59" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="W59" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="X59" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="Y59" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="Z59" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC59" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="AD59" s="7"/>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="7"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="7"/>
+      <c r="AK59" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="3">
+        <v>2025091469</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="3">
+        <v>5291</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N60" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O60" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S60" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T60" s="3">
+        <v>1</v>
+      </c>
+      <c r="U60" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V60" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="W60" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="X60" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y60" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z60" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC60" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="AD60" s="3"/>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="3"/>
+      <c r="AG60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3"/>
+      <c r="AK60" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="7">
+        <v>2025091559</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7">
+        <v>3751</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="R61" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T61" s="7">
+        <v>1</v>
+      </c>
+      <c r="U61" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V61" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="W61" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="X61" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC61" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="AD61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="7"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK61" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="3">
+        <v>2025091585</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3">
+        <v>3243</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S62" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T62" s="3">
+        <v>1</v>
+      </c>
+      <c r="U62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V62" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="W62" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="X62" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC62" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE62" s="3"/>
+      <c r="AF62" s="3"/>
+      <c r="AG62" s="3"/>
+      <c r="AH62" s="3"/>
+      <c r="AI62" s="3"/>
+      <c r="AJ62" s="3"/>
+      <c r="AK62" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="7">
+        <v>2025091591</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7">
+        <v>3137</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T63" s="7">
+        <v>1</v>
+      </c>
+      <c r="U63" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="W63" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="X63" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC63" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD63" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="7"/>
+      <c r="AK63" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09111716
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$78</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="525">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-10  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="664">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-11  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1632,6 +1632,42 @@
 </t>
   </si>
   <si>
+    <t>E2759114090901</t>
+  </si>
+  <si>
+    <t>三重仁化店</t>
+  </si>
+  <si>
+    <t>2025-09-09 15:02:23</t>
+  </si>
+  <si>
+    <t>螢幕聲音異常</t>
+  </si>
+  <si>
+    <t>店長告知SC(LCD)逼放監視器時聲音僅有單邊，另一邊都沒有聲音，已有將電源關閉重開線路重新拔插仍無法排除......還請台芝到店協助(監視器喇叭聲音)</t>
+  </si>
+  <si>
+    <t>THILF02759</t>
+  </si>
+  <si>
+    <t>2025-09-09 15:16:52</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:22:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:52:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 19:16:00</t>
+  </si>
+  <si>
+    <t>原本監視器的喇叭無聲音，
+改插音源線至螢幕一樣沒聲音，
+換新螢幕一樣沒聲音，
+請現場人員叫修監視器廠商處理</t>
+  </si>
+  <si>
     <t>2025-09-09 18:02:29</t>
   </si>
   <si>
@@ -1644,6 +1680,71 @@
     <t>PMQ3+PEP安裝完成</t>
   </si>
   <si>
+    <t>14856114090901</t>
+  </si>
+  <si>
+    <t>2025-09-09 18:34:51</t>
+  </si>
+  <si>
+    <t>HLF3</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET QRcode掃描器</t>
+  </si>
+  <si>
+    <t>F301</t>
+  </si>
+  <si>
+    <t>門市反應MMK QRCODE掃描器掃描條碼都會異常，掃描手機QRCODE的時候都會有嗶聲，但都會顯示延遲或是錯誤，更多時候都沒有讀取到，MMK已有重新開機仍無法排除，已造成門市作業不便...........還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-09 18:37:03</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 22:37:00</t>
+  </si>
+  <si>
+    <t>更換掃描器</t>
+  </si>
+  <si>
+    <t>E4228114091001</t>
+  </si>
+  <si>
+    <t>新莊頭前公園</t>
+  </si>
+  <si>
+    <t>2025-09-10 07:38:44</t>
+  </si>
+  <si>
+    <t>門市TM1(TCX800)無電源反應電源燈未亮，門市已有重新拔插線路休息、更換插座仍無法開機....須請台芝到店協助(機台插座插了無法使用)
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認今日尚未清帳，入帳日09/10有交易</t>
+  </si>
+  <si>
+    <t>THILF04228</t>
+  </si>
+  <si>
+    <t>2025-09-10 09:07:14</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 13:07:00</t>
+  </si>
+  <si>
+    <t>重插變壓器電源線</t>
+  </si>
+  <si>
     <t>2025-09-10 10:01:35</t>
   </si>
   <si>
@@ -1663,6 +1764,350 @@
   </si>
   <si>
     <t>2025-09-10 10:30:00</t>
+  </si>
+  <si>
+    <t>13380114091001</t>
+  </si>
+  <si>
+    <t>北縣莊勝店</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:30:59</t>
+  </si>
+  <si>
+    <t>TM1發票機(BSC10II)門市告知兩筆皆為交班後的第一筆交易，僅出一小截空白，與門市確認當下發票機燈號正常TM未出現異常訊息，未操作任何基本排除後續出發票正常，此兩筆都已作廢重結，發票機為二代（BSC10II)，經HIPOS查看:eventlog無異常，發票檔內有此張發票，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。與門市確認這幾天頻繁發生....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03380</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:35:39</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:35:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上8155004157
+換下8155004451</t>
+  </si>
+  <si>
+    <t>12042114091001</t>
+  </si>
+  <si>
+    <t>三重中央北店</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:42:15</t>
+  </si>
+  <si>
+    <t>門市反應TM2掃描器(HC76-TR)清帳後都會跳出COMPORT偵測異常，點選清除後，出現：COMPORT偵測異常，請按[清除]後，退到登入頁面，按下[版本更新]，自動重啟系統，或撥打0800客服報修11111，因頻繁發生門市告知已造成困擾。經HIPOS查詢:與開發確認，出現回主畫面出現COMPORT偵測異常，請按[清除]後，退到登入頁面，按下[版本更新]為系統與CCD之間連線問題，煩請轉派台芝到店檢查相關設備及線路。...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02042</t>
+  </si>
+  <si>
+    <t>2025-09-10 10:45:54</t>
+  </si>
+  <si>
+    <t>2025-09-10 12:22:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:45:00</t>
+  </si>
+  <si>
+    <t>門市表示只有發生在交班之後，現場確認掃槍無異狀，依然更換備品
+更換掃描槍
+換下8119012710
+換上8119012934</t>
+  </si>
+  <si>
+    <t>14029114091001</t>
+  </si>
+  <si>
+    <t>三重龍濱店</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:05:05</t>
+  </si>
+  <si>
+    <t>門市TM1 CCD掃描器(HC56II-TR)無法刷讀，有亮燈有逼聲，已有執行校正表單以及TM重啟仍異常...請台芝到店協助，客服VNC查看輸入顯示鼠標正常，.....還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04029</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:07:53</t>
+  </si>
+  <si>
+    <t>2025-09-11 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 15:07:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119008703
+換上8119012935</t>
+  </si>
+  <si>
+    <t>13243114091001</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:31:28</t>
+  </si>
+  <si>
+    <t>門市反應SC螢幕(LCD)有水波紋，VNC畫面正常，請門市重新插拔螢幕線路後仍異常，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:33:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 14:43:00</t>
+  </si>
+  <si>
+    <t>2025-09-10 15:13:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 15:33:00</t>
+  </si>
+  <si>
+    <t>取消叫修</t>
+  </si>
+  <si>
+    <t>客戶取消</t>
+  </si>
+  <si>
+    <t>1D161114091001</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:43:24</t>
+  </si>
+  <si>
+    <t>門市告知TM2（BSC10II）無正常出發票，完全無印出，當下TM未出現異常訊息，未操作任何基本排除後續交易發票出紙正常，發票機為二代（BSC10II），後續門市已重新交易有印出發票。經HIPOS查看一般交易未印出發票 eventlog有報錯拒絕存取路徑，查看9/4未列印出退瓶帳條，如頻繁發生建議轉派台芝到店更換相關設備。...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-10 11:45:01</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 15:45:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上：8155004438
+換下：8155006284</t>
+  </si>
+  <si>
+    <t>13601114091003</t>
+  </si>
+  <si>
+    <t>北縣重富店</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:30:47</t>
+  </si>
+  <si>
+    <t>TM1（BSC10II）門市告知TM1清帳後有印出帳條但未印出退瓶，與門市確認當下發票機燈號正常，TM未出現異常訊息，未操作任何基本排除後續交易發票出紙正常，發票機為二代（BSC10II），因收據無法補印。總公司規定門市應落實張貼交回，遺失此憑證將視為短匯(會扣錢)經hipos確認:退瓶有入帳，收據檔內有此張退瓶收據，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。與門市確認頻繁發生....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03601</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:36:46</t>
+  </si>
+  <si>
+    <t>2025-09-11 09:34:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 10:04:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 17:36:00</t>
+  </si>
+  <si>
+    <t>檢測發票機狀況皆為正常，依然更換備品
+換下8155005464
+換上8155004449</t>
+  </si>
+  <si>
+    <t>13601114091004</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:31:09</t>
+  </si>
+  <si>
+    <t>TM2（BSC10II）門市告知TM2清帳後有印出帳條但未印出退瓶，與門市確認當下發票機燈號正常，TM未出現異常訊息，未操作任何基本排除後續交易發票出紙正常，發票機為二代（BSC10II），因收據無法補印。總公司規定門市應落實張貼交回，遺失此憑證將視為短匯(會扣錢)經hipos確認:退瓶有入帳，收據檔內有此張退瓶收據，判斷此非tm軟體障礙，請門市再觀察，如頻繁發生建議轉派台芝到店檢查相關設備及線路。與門市確認頻繁發生....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-10 13:37:26</t>
+  </si>
+  <si>
+    <t>2025-09-11 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 10:07:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 17:37:00</t>
+  </si>
+  <si>
+    <t>檢測發票機狀況皆為正常，依然更換備品
+換下8155005465
+換上8155004448</t>
+  </si>
+  <si>
+    <t>E5354114091001</t>
+  </si>
+  <si>
+    <t>蘆洲希望店</t>
+  </si>
+  <si>
+    <t>2025-09-10 14:22:15</t>
+  </si>
+  <si>
+    <t>HL59</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET熱感機T70II</t>
+  </si>
+  <si>
+    <t>印字不清</t>
+  </si>
+  <si>
+    <t>門市反應LIFE ET熱感機(T70II)印出的小白單明顯有一條豎著的空白線條，已請門市嘗試重裝紙捲、重啟熱感機電源，清潔出票口仍異常，需請台芝到店協助(條碼不完整)</t>
+  </si>
+  <si>
+    <t>THILF05354</t>
+  </si>
+  <si>
+    <t>2025-09-10 14:27:30</t>
+  </si>
+  <si>
+    <t>2025-09-11 15:32:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 16:02:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 18:27:00</t>
+  </si>
+  <si>
+    <t>清除熱感頭上異物，測試列印可正常</t>
+  </si>
+  <si>
+    <t>1D161114091002</t>
+  </si>
+  <si>
+    <t>2025-09-10 17:33:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市TM1(TCX800)觸控異常鼠標亂點飄移，VNC查看鼠標飄移嚴重無法操作觸控校正重啟後仍異常，無張貼文宣.....須請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>2025-09-10 17:35:32</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:46:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 15:16:00</t>
+  </si>
+  <si>
+    <t>2025-09-11 21:35:00</t>
+  </si>
+  <si>
+    <t>報修櫃號錯誤，取消報修</t>
+  </si>
+  <si>
+    <t>E2209114091101</t>
+  </si>
+  <si>
+    <t>三重圖書館</t>
+  </si>
+  <si>
+    <t>2025-09-11 11:30:04</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)抽屜無法正常關閉，都需喬一定的角度才可正常關閉(抽屜顏色:白色/鑰匙孔位子:中/鑰匙孔無編號)..請台芝到店協助(1號機抽屜無法正常關 需兩次很大聲才能關起)</t>
+  </si>
+  <si>
+    <t>THILF02209</t>
+  </si>
+  <si>
+    <t>2025-09-11 11:40:53</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:33:00</t>
+  </si>
+  <si>
+    <t>2025-09-12 15:40:00</t>
+  </si>
+  <si>
+    <t>更換錢櫃
+換下81Z1000766
+換上81Z1003659</t>
+  </si>
+  <si>
+    <t>E2209114091102</t>
+  </si>
+  <si>
+    <t>2025-09-11 11:31:40</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控不良，靠近會員載具的區域很難按，都需按好幾下才有反應，已嘗試執行觸控校正仍無改善..請台芝到店協助(2號機面板螢幕無法定位  會飄逸)
+9/11 11:38 協助門市執行觸控校正，稍晚去電確認..吳</t>
+  </si>
+  <si>
+    <t>2025-09-11 11:50:20</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:32:00</t>
+  </si>
+  <si>
+    <t>2025-09-12 15:50:00</t>
+  </si>
+  <si>
+    <t>更換TM主機，無更換硬碟
+換下818500534
+換上818500353</t>
+  </si>
+  <si>
+    <t>1D161114091101</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:56:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市TM2(TCX800)觸控異常鼠標亂點飄移，VNC查看鼠標飄移嚴重無法操作觸控校正重啟後仍異常，無張貼文宣.....須請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>2025-09-11 14:57:20</t>
+  </si>
+  <si>
+    <t>2025-09-11 15:25:00</t>
+  </si>
+  <si>
+    <t>2025-09-12 18:57:00</t>
+  </si>
+  <si>
+    <t>到場後詢問門市表示機器已無問題，
+並且報修櫃號為TM2非TM1
+現場觀察半個小時以上觸控均無異狀
+1.嘗試交易-正常
+2.登出登入-正常
+3.重新開機-正常</t>
   </si>
 </sst>
 </file>
@@ -2076,10 +2521,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK63"/>
+  <dimension ref="A1:AK78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="AC75" sqref="AC75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7336,32 +7781,52 @@
         <v>59</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C61" s="7">
-        <v>2025091559</v>
-      </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
+        <v>2025091531</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F61" s="7">
-        <v>3751</v>
+        <v>2759</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>405</v>
+        <v>515</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="7"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L61" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="N61" s="7">
+        <v>2503</v>
+      </c>
+      <c r="O61" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="P61" s="9" t="s">
+        <v>518</v>
+      </c>
       <c r="Q61" s="7" t="s">
-        <v>411</v>
+        <v>519</v>
       </c>
       <c r="R61" s="7" t="s">
         <v>51</v>
@@ -7376,36 +7841,34 @@
         <v>53</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="W61" s="7" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="X61" s="7" t="s">
-        <v>516</v>
-      </c>
-      <c r="Y61" s="7"/>
+        <v>522</v>
+      </c>
+      <c r="Y61" s="7" t="s">
+        <v>523</v>
+      </c>
       <c r="Z61" s="7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AA61" s="7"/>
       <c r="AB61" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC61" s="9" t="s">
-        <v>517</v>
-      </c>
-      <c r="AD61" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="AD61" s="7"/>
       <c r="AE61" s="7"/>
       <c r="AF61" s="7"/>
       <c r="AG61" s="7"/>
       <c r="AH61" s="7"/>
       <c r="AI61" s="7"/>
-      <c r="AJ61" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ61" s="7"/>
       <c r="AK61" s="7" t="s">
         <v>60</v>
       </c>
@@ -7418,18 +7881,18 @@
         <v>135</v>
       </c>
       <c r="C62" s="3">
-        <v>2025091585</v>
+        <v>2025091559</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3">
-        <v>3243</v>
+        <v>3751</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>450</v>
+        <v>405</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>396</v>
+        <v>212</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
@@ -7440,13 +7903,13 @@
       <c r="O62" s="4"/>
       <c r="P62" s="10"/>
       <c r="Q62" s="3" t="s">
-        <v>456</v>
+        <v>411</v>
       </c>
       <c r="R62" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="T62" s="3">
         <v>1</v>
@@ -7455,24 +7918,24 @@
         <v>53</v>
       </c>
       <c r="V62" s="3" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="W62" s="3" t="s">
-        <v>463</v>
+        <v>526</v>
       </c>
       <c r="X62" s="3" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="Y62" s="3"/>
       <c r="Z62" s="3">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="AA62" s="3"/>
       <c r="AB62" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC62" s="10" t="s">
-        <v>141</v>
+        <v>528</v>
       </c>
       <c r="AD62" s="3" t="s">
         <v>60</v>
@@ -7482,7 +7945,9 @@
       <c r="AG62" s="3"/>
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
-      <c r="AJ62" s="3"/>
+      <c r="AJ62" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AK62" s="3" t="s">
         <v>60</v>
       </c>
@@ -7492,32 +7957,52 @@
         <v>61</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C63" s="7">
-        <v>2025091591</v>
-      </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
+        <v>2025091560</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F63" s="7">
-        <v>3137</v>
+        <v>4856</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>520</v>
+        <v>184</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="7"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="8"/>
+        <v>80</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K63" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="M63" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="N63" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="O63" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P63" s="9" t="s">
+        <v>534</v>
+      </c>
       <c r="Q63" s="7" t="s">
-        <v>522</v>
+        <v>190</v>
       </c>
       <c r="R63" s="7" t="s">
         <v>51</v>
@@ -7532,15 +8017,17 @@
         <v>53</v>
       </c>
       <c r="V63" s="7" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="W63" s="7" t="s">
-        <v>519</v>
+        <v>536</v>
       </c>
       <c r="X63" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="Y63" s="7"/>
+        <v>537</v>
+      </c>
+      <c r="Y63" s="7" t="s">
+        <v>538</v>
+      </c>
       <c r="Z63" s="7">
         <v>0.3</v>
       </c>
@@ -7548,12 +8035,10 @@
       <c r="AB63" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC63" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD63" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC63" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="AD63" s="7"/>
       <c r="AE63" s="7"/>
       <c r="AF63" s="7"/>
       <c r="AG63" s="7"/>
@@ -7561,6 +8046,1421 @@
       <c r="AI63" s="7"/>
       <c r="AJ63" s="7"/>
       <c r="AK63" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="3">
+        <v>2025091568</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="3">
+        <v>4228</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N64" s="3">
+        <v>2306</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S64" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T64" s="3">
+        <v>1</v>
+      </c>
+      <c r="U64" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V64" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="W64" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="X64" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="Y64" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="Z64" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC64" s="10" t="s">
+        <v>549</v>
+      </c>
+      <c r="AD64" s="3"/>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="3"/>
+      <c r="AG64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3"/>
+      <c r="AK64" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:37">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2025091585</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7">
+        <v>3243</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="R65" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S65" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T65" s="7">
+        <v>1</v>
+      </c>
+      <c r="U65" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V65" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="W65" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="X65" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC65" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD65" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7"/>
+      <c r="AK65" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2025091591</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3">
+        <v>3137</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T66" s="3">
+        <v>1</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V66" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC66" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD66" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="3"/>
+      <c r="AG66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3"/>
+      <c r="AK66" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" s="7">
+        <v>2025091593</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="7">
+        <v>3380</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K67" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L67" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N67" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O67" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P67" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q67" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="R67" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S67" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T67" s="7">
+        <v>1</v>
+      </c>
+      <c r="U67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V67" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="W67" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="X67" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="Y67" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="Z67" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC67" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="AD67" s="7"/>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="7"/>
+      <c r="AG67" s="7"/>
+      <c r="AH67" s="7"/>
+      <c r="AI67" s="7"/>
+      <c r="AJ67" s="7"/>
+      <c r="AK67" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" s="3">
+        <v>2025091596</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F68" s="3">
+        <v>2042</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P68" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T68" s="3">
+        <v>1</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V68" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="W68" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="X68" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y68" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z68" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC68" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="AD68" s="3"/>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="7">
+        <v>2025091602</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="7">
+        <v>4029</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K69" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M69" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N69" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O69" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P69" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q69" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="R69" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T69" s="7">
+        <v>1</v>
+      </c>
+      <c r="U69" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V69" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="W69" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="X69" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="Y69" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="Z69" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC69" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="AD69" s="7"/>
+      <c r="AE69" s="7"/>
+      <c r="AF69" s="7"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="7"/>
+      <c r="AI69" s="7"/>
+      <c r="AJ69" s="7"/>
+      <c r="AK69" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="3">
+        <v>2025091610</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="3">
+        <v>3243</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="N70" s="3">
+        <v>2501</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="P70" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="Q70" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T70" s="3">
+        <v>1</v>
+      </c>
+      <c r="U70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V70" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="W70" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="X70" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="Y70" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="Z70" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA70" s="3"/>
+      <c r="AB70" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="AC70" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="AD70" s="3"/>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="3"/>
+      <c r="AG70" s="3"/>
+      <c r="AH70" s="3"/>
+      <c r="AI70" s="3"/>
+      <c r="AJ70" s="3"/>
+      <c r="AK70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:37">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="7">
+        <v>2025091612</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K71" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M71" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N71" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O71" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P71" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q71" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="R71" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S71" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T71" s="7">
+        <v>1</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V71" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="W71" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="X71" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="Y71" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="Z71" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC71" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="AD71" s="7"/>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="7"/>
+      <c r="AG71" s="7"/>
+      <c r="AH71" s="7"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="7"/>
+      <c r="AK71" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:37">
+      <c r="A72" s="3">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="3">
+        <v>2025091617</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="3">
+        <v>3601</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N72" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P72" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q72" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T72" s="3">
+        <v>1</v>
+      </c>
+      <c r="U72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V72" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="W72" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="X72" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="Y72" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="Z72" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA72" s="3"/>
+      <c r="AB72" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC72" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="AD72" s="3"/>
+      <c r="AE72" s="3"/>
+      <c r="AF72" s="3"/>
+      <c r="AG72" s="3"/>
+      <c r="AH72" s="3"/>
+      <c r="AI72" s="3"/>
+      <c r="AJ72" s="3"/>
+      <c r="AK72" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:37">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="7">
+        <v>2025091618</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="7">
+        <v>3601</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K73" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L73" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M73" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N73" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O73" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P73" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q73" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="R73" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S73" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T73" s="7">
+        <v>1</v>
+      </c>
+      <c r="U73" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V73" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="W73" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="X73" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y73" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="Z73" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA73" s="7"/>
+      <c r="AB73" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC73" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="AD73" s="7"/>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="7"/>
+      <c r="AG73" s="7"/>
+      <c r="AH73" s="7"/>
+      <c r="AI73" s="7"/>
+      <c r="AJ73" s="7"/>
+      <c r="AK73" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:37">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" s="3">
+        <v>2025091634</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F74" s="3">
+        <v>5354</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="N74" s="3">
+        <v>5902</v>
+      </c>
+      <c r="O74" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="P74" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="Q74" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T74" s="3">
+        <v>1</v>
+      </c>
+      <c r="U74" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V74" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="W74" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="X74" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="Y74" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="Z74" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA74" s="3"/>
+      <c r="AB74" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC74" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD74" s="3"/>
+      <c r="AE74" s="3"/>
+      <c r="AF74" s="3"/>
+      <c r="AG74" s="3"/>
+      <c r="AH74" s="3"/>
+      <c r="AI74" s="3"/>
+      <c r="AJ74" s="3"/>
+      <c r="AK74" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="7">
+        <v>2025091738</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N75" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O75" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P75" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q75" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="R75" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T75" s="7">
+        <v>1</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V75" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="W75" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="X75" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="Y75" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="Z75" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC75" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="AD75" s="7"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
+      <c r="AG75" s="7"/>
+      <c r="AH75" s="7"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="7"/>
+      <c r="AK75" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2025091777</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" s="3">
+        <v>2209</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N76" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q76" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S76" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T76" s="3">
+        <v>1</v>
+      </c>
+      <c r="U76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V76" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="W76" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="X76" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="Y76" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="Z76" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC76" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="AD76" s="3"/>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="3"/>
+      <c r="AG76" s="3"/>
+      <c r="AH76" s="3"/>
+      <c r="AI76" s="3"/>
+      <c r="AJ76" s="3"/>
+      <c r="AK76" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="7">
+        <v>2025091782</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="7">
+        <v>2209</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="K77" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L77" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M77" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N77" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O77" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P77" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="Q77" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="R77" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T77" s="7">
+        <v>1</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V77" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="W77" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="X77" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="Y77" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="Z77" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC77" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="AD77" s="7"/>
+      <c r="AE77" s="7"/>
+      <c r="AF77" s="7"/>
+      <c r="AG77" s="7"/>
+      <c r="AH77" s="7"/>
+      <c r="AI77" s="7"/>
+      <c r="AJ77" s="7"/>
+      <c r="AK77" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" s="3">
+        <v>2025091812</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N78" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P78" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="Q78" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T78" s="3">
+        <v>1</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="X78" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y78" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="Z78" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC78" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="AD78" s="3"/>
+      <c r="AE78" s="3"/>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AI78" s="3"/>
+      <c r="AJ78" s="3"/>
+      <c r="AK78" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09121752
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$79</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="664">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-11  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="669">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-12  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2108,6 +2108,21 @@
 1.嘗試交易-正常
 2.登出登入-正常
 3.重新開機-正常</t>
+  </si>
+  <si>
+    <t>三重金陵店</t>
+  </si>
+  <si>
+    <t>THILF03359</t>
+  </si>
+  <si>
+    <t>2025-09-12 13:54:09</t>
+  </si>
+  <si>
+    <t>2025-09-12 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-12 13:53:00</t>
   </si>
 </sst>
 </file>
@@ -2521,10 +2536,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK78"/>
+  <dimension ref="A1:AK79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC75" sqref="AC75"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9413,7 +9428,7 @@
       <c r="O78" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="P78" s="4" t="s">
+      <c r="P78" s="10" t="s">
         <v>659</v>
       </c>
       <c r="Q78" s="3" t="s">
@@ -9450,7 +9465,7 @@
       <c r="AB78" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC78" s="4" t="s">
+      <c r="AC78" s="10" t="s">
         <v>663</v>
       </c>
       <c r="AD78" s="3"/>
@@ -9461,6 +9476,83 @@
       <c r="AI78" s="3"/>
       <c r="AJ78" s="3"/>
       <c r="AK78" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:37">
+      <c r="A79" s="7">
+        <v>77</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79" s="7">
+        <v>2025091881</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7">
+        <v>3359</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="8"/>
+      <c r="Q79" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="R79" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T79" s="7">
+        <v>1</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V79" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="W79" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="X79" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="Y79" s="7"/>
+      <c r="Z79" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC79" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD79" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="7"/>
+      <c r="AG79" s="7"/>
+      <c r="AH79" s="7"/>
+      <c r="AI79" s="7"/>
+      <c r="AJ79" s="7"/>
+      <c r="AK79" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09151626
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$82</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="669">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-12  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="692">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-15  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2123,6 +2123,82 @@
   </si>
   <si>
     <t>2025-09-12 13:53:00</t>
+  </si>
+  <si>
+    <t>E2209114091501</t>
+  </si>
+  <si>
+    <t>2025-09-15 07:18:50</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)刷讀商品後左邊刪除鍵無法按壓，已嘗試執行觸控校正仍異常，09/11 台芝到店更換TM主機..請台芝到店協助(2號機新換螢幕當機刷的商品無法安取消)
+09/15  09:11  請協助門市觸控校正，稍晚去電確認...廖</t>
+  </si>
+  <si>
+    <t>2025-09-15 09:34:52</t>
+  </si>
+  <si>
+    <t>2025-09-15 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-15 11:58:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:34:00</t>
+  </si>
+  <si>
+    <t>更換主機，無更換硬碟
+換下8185000353
+換上8185000186</t>
+  </si>
+  <si>
+    <t>13751114091501</t>
+  </si>
+  <si>
+    <t>2025-09-15 09:43:23</t>
+  </si>
+  <si>
+    <t>F602</t>
+  </si>
+  <si>
+    <t>無法讀卡</t>
+  </si>
+  <si>
+    <t>門市反應TM1多卡機QP3000E無法使用悠遊卡、一卡通、愛金卡，出現訊息Unknown message! ，協助門市TM點選版更後悠遊卡機重開成功，測試交易仍顯示此訊息...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-15 09:44:23</t>
+  </si>
+  <si>
+    <t>2025-09-15 14:35:00</t>
+  </si>
+  <si>
+    <t>2025-09-15 15:05:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:44:00</t>
+  </si>
+  <si>
+    <t>更換多卡機
+換下8183003227
+換上8183000568</t>
+  </si>
+  <si>
+    <t>新莊福祐店</t>
+  </si>
+  <si>
+    <t>THILF03999</t>
+  </si>
+  <si>
+    <t>2025-09-15 15:34:06</t>
+  </si>
+  <si>
+    <t>2025-09-15 15:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">回裝作業已完成
+mmk安裝螺帽x4
+</t>
   </si>
 </sst>
 </file>
@@ -2536,10 +2612,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK79"/>
+  <dimension ref="A1:AK82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="AC79" sqref="AC79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9507,7 +9583,7 @@
       <c r="M79" s="8"/>
       <c r="N79" s="7"/>
       <c r="O79" s="8"/>
-      <c r="P79" s="8"/>
+      <c r="P79" s="9"/>
       <c r="Q79" s="7" t="s">
         <v>665</v>
       </c>
@@ -9540,7 +9616,7 @@
       <c r="AB79" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC79" s="8" t="s">
+      <c r="AC79" s="9" t="s">
         <v>141</v>
       </c>
       <c r="AD79" s="7" t="s">
@@ -9553,6 +9629,277 @@
       <c r="AI79" s="7"/>
       <c r="AJ79" s="7"/>
       <c r="AK79" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:37">
+      <c r="A80" s="3">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2025091943</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F80" s="3">
+        <v>2209</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N80" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="Q80" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S80" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T80" s="3">
+        <v>1</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V80" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="X80" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="Y80" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="Z80" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC80" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="AD80" s="3"/>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AI80" s="3"/>
+      <c r="AJ80" s="3"/>
+      <c r="AK80" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:37">
+      <c r="A81" s="7">
+        <v>79</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2025091945</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="7">
+        <v>3751</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I81" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="J81" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K81" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L81" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M81" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="N81" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="O81" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="P81" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q81" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="R81" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S81" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T81" s="7">
+        <v>1</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V81" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="W81" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="X81" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="Y81" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="Z81" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC81" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="AD81" s="7"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7"/>
+      <c r="AK81" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37">
+      <c r="A82" s="3">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C82" s="3">
+        <v>2025092032</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3">
+        <v>3999</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S82" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T82" s="3">
+        <v>1</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3">
+        <v>5</v>
+      </c>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC82" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="AD82" s="3"/>
+      <c r="AE82" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="3"/>
+      <c r="AH82" s="3"/>
+      <c r="AI82" s="3"/>
+      <c r="AJ82" s="3"/>
+      <c r="AK82" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09161537
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$82</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$89</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="692">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-15  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="732">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-16  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2199,6 +2199,126 @@
     <t xml:space="preserve">回裝作業已完成
 mmk安裝螺帽x4
 </t>
+  </si>
+  <si>
+    <t>D767</t>
+  </si>
+  <si>
+    <t>板橋寶翠店</t>
+  </si>
+  <si>
+    <t>THILF0D767</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:21:29</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:15:00</t>
+  </si>
+  <si>
+    <t>北縣板嘉店</t>
+  </si>
+  <si>
+    <t>THILF02746</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:58:47</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:20:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:43:00</t>
+  </si>
+  <si>
+    <t>板橋雙十店</t>
+  </si>
+  <si>
+    <t>THILF02221</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:08:44</t>
+  </si>
+  <si>
+    <t>2025-09-16 12:46:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:08:00</t>
+  </si>
+  <si>
+    <t>板橋藝文中心</t>
+  </si>
+  <si>
+    <t>THILF03399</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:44:45</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:15:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:42:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:08:25</t>
+  </si>
+  <si>
+    <t>2025-09-16 13:50:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:06:00</t>
+  </si>
+  <si>
+    <t>板橋江子翠站</t>
+  </si>
+  <si>
+    <t>THILF02069</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:28:31</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:28:00</t>
+  </si>
+  <si>
+    <t>14680114091601</t>
+  </si>
+  <si>
+    <t>板橋江寧店</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:58:58</t>
+  </si>
+  <si>
+    <t>HUB週期維護</t>
+  </si>
+  <si>
+    <t>2025年07月份 hub調查異常:PING91不通無法連線HUB，其他線路正常</t>
+  </si>
+  <si>
+    <t>THILF04680</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:59:17</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:22:00</t>
+  </si>
+  <si>
+    <t>2025-09-16 14:59:00</t>
+  </si>
+  <si>
+    <t>2025-09-17 18:59:00</t>
+  </si>
+  <si>
+    <t>HUB  ping91不通已排除</t>
   </si>
 </sst>
 </file>
@@ -2612,10 +2732,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK82"/>
+  <dimension ref="A1:AK89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC79" sqref="AC79"/>
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9854,7 +9974,7 @@
       <c r="M82" s="4"/>
       <c r="N82" s="3"/>
       <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
+      <c r="P82" s="10"/>
       <c r="Q82" s="3" t="s">
         <v>688</v>
       </c>
@@ -9887,7 +10007,7 @@
       <c r="AB82" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC82" s="4" t="s">
+      <c r="AC82" s="10" t="s">
         <v>691</v>
       </c>
       <c r="AD82" s="3"/>
@@ -9900,6 +10020,565 @@
       <c r="AI82" s="3"/>
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37">
+      <c r="A83" s="7">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2025092112</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="R83" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T83" s="7">
+        <v>1</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V83" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="W83" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="X83" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC83" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
+      <c r="AI83" s="7"/>
+      <c r="AJ83" s="7"/>
+      <c r="AK83" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37">
+      <c r="A84" s="3">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" s="3">
+        <v>2025092117</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3">
+        <v>2746</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T84" s="3">
+        <v>1</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V84" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA84" s="3"/>
+      <c r="AB84" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC84" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD84" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE84" s="3"/>
+      <c r="AF84" s="3"/>
+      <c r="AG84" s="3"/>
+      <c r="AH84" s="3"/>
+      <c r="AI84" s="3"/>
+      <c r="AJ84" s="3"/>
+      <c r="AK84" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:37">
+      <c r="A85" s="7">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2025092118</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7">
+        <v>2221</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="9"/>
+      <c r="Q85" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="R85" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S85" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T85" s="7">
+        <v>1</v>
+      </c>
+      <c r="U85" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V85" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="W85" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="X85" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC85" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD85" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="7"/>
+      <c r="AH85" s="7"/>
+      <c r="AI85" s="7"/>
+      <c r="AJ85" s="7"/>
+      <c r="AK85" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:37">
+      <c r="A86" s="3">
+        <v>84</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C86" s="3">
+        <v>2025092124</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3">
+        <v>3399</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="10"/>
+      <c r="Q86" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="R86" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S86" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T86" s="3">
+        <v>1</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V86" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="W86" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="X86" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC86" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD86" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="3"/>
+      <c r="AI86" s="3"/>
+      <c r="AJ86" s="3"/>
+      <c r="AK86" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37">
+      <c r="A87" s="7">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="7">
+        <v>2025092128</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7">
+        <v>2224</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="7"/>
+      <c r="O87" s="8"/>
+      <c r="P87" s="9"/>
+      <c r="Q87" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="R87" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S87" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T87" s="7">
+        <v>1</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V87" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="W87" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="X87" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="Y87" s="7"/>
+      <c r="Z87" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC87" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD87" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="7"/>
+      <c r="AH87" s="7"/>
+      <c r="AI87" s="7"/>
+      <c r="AJ87" s="7"/>
+      <c r="AK87" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:37">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88" s="3">
+        <v>2025092137</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3">
+        <v>2069</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S88" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T88" s="3">
+        <v>1</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V88" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="X88" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="Y88" s="3"/>
+      <c r="Z88" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC88" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD88" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="3"/>
+      <c r="AG88" s="3"/>
+      <c r="AH88" s="3"/>
+      <c r="AI88" s="3"/>
+      <c r="AJ88" s="3"/>
+      <c r="AK88" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:37">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="7">
+        <v>2025092145</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="7">
+        <v>4680</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K89" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="M89" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="N89" s="7">
+        <v>3404</v>
+      </c>
+      <c r="O89" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="P89" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="Q89" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T89" s="7">
+        <v>1</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="W89" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="X89" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="Y89" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="Z89" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC89" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="AD89" s="7"/>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="7"/>
+      <c r="AH89" s="7"/>
+      <c r="AI89" s="7"/>
+      <c r="AJ89" s="7"/>
+      <c r="AK89" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09171436
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$89</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$92</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="732">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-16  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="749">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-17  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2319,6 +2319,57 @@
   </si>
   <si>
     <t>HUB  ping91不通已排除</t>
+  </si>
+  <si>
+    <t>E4282114091601</t>
+  </si>
+  <si>
+    <t>2025-09-16 16:20:36</t>
+  </si>
+  <si>
+    <t>門市反映MMK熱感機(T70-II)列印出的單據到兩台TM都無法刷讀，門市已有重裝紙捲重開機仍異常...須請台芝到店協助(沒辦法操作)</t>
+  </si>
+  <si>
+    <t>2025-09-16 16:34:11</t>
+  </si>
+  <si>
+    <t>2025-09-17 13:31:00</t>
+  </si>
+  <si>
+    <t>2025-09-17 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-17 20:34:00</t>
+  </si>
+  <si>
+    <t>清潔t70</t>
+  </si>
+  <si>
+    <t>2025-09-17 10:40:36</t>
+  </si>
+  <si>
+    <t>2025-09-17 10:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-17 10:40:00</t>
+  </si>
+  <si>
+    <t>蘆洲中山一</t>
+  </si>
+  <si>
+    <t>THILF03929</t>
+  </si>
+  <si>
+    <t>2025-09-17 13:42:12</t>
+  </si>
+  <si>
+    <t>2025-09-17 13:25:00</t>
+  </si>
+  <si>
+    <t>2025-09-17 13:50:00</t>
+  </si>
+  <si>
+    <t>裝潢回裝完成</t>
   </si>
 </sst>
 </file>
@@ -2732,10 +2783,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK89"/>
+  <dimension ref="A1:AK92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A89" sqref="A89"/>
+      <selection activeCell="AC89" sqref="AC89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10531,7 +10582,7 @@
       <c r="O89" s="8" t="s">
         <v>724</v>
       </c>
-      <c r="P89" s="8" t="s">
+      <c r="P89" s="9" t="s">
         <v>725</v>
       </c>
       <c r="Q89" s="7" t="s">
@@ -10568,7 +10619,7 @@
       <c r="AB89" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC89" s="8" t="s">
+      <c r="AC89" s="9" t="s">
         <v>731</v>
       </c>
       <c r="AD89" s="7"/>
@@ -10579,6 +10630,255 @@
       <c r="AI89" s="7"/>
       <c r="AJ89" s="7"/>
       <c r="AK89" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2025092221</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="3">
+        <v>4282</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="N90" s="3">
+        <v>5902</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>734</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2025092284</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7">
+        <v>3999</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC91" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD91" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2025092314</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T92" s="3">
+        <v>1</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="Y92" s="3"/>
+      <c r="Z92" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3"/>
+      <c r="AC92" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="AD92" s="3"/>
+      <c r="AE92" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+      <c r="AJ92" s="3"/>
+      <c r="AK92" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09181531
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$92</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$97</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="749">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-17  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="785">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-18  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2370,6 +2370,117 @@
   </si>
   <si>
     <t>裝潢回裝完成</t>
+  </si>
+  <si>
+    <t>ED620114091801</t>
+  </si>
+  <si>
+    <t>D620</t>
+  </si>
+  <si>
+    <t>三重福隆店</t>
+  </si>
+  <si>
+    <t>2025-09-18 00:12:53</t>
+  </si>
+  <si>
+    <t>門市反應TM1-CCD掃描器(HC76-TR)無電源反應，已確認後方線路無鬆脫，重啟TM仍異常..請台芝到店協助(掃描器無紅光，無法掃描)
+9/18 09:02 致電門市未接..吳</t>
+  </si>
+  <si>
+    <t>THILF0D620</t>
+  </si>
+  <si>
+    <t>2025-09-18 09:14:36</t>
+  </si>
+  <si>
+    <t>2025-09-18 13:21:00</t>
+  </si>
+  <si>
+    <t>2025-09-18 13:51:00</t>
+  </si>
+  <si>
+    <t>2025-09-19 13:14:00</t>
+  </si>
+  <si>
+    <t>TX800的IO卡無反應，更換IO卡後測試正常</t>
+  </si>
+  <si>
+    <t>1D191114091801</t>
+  </si>
+  <si>
+    <t>D191</t>
+  </si>
+  <si>
+    <t>三重興德店</t>
+  </si>
+  <si>
+    <t>2025-09-18 10:03:23</t>
+  </si>
+  <si>
+    <t>門市反應TM1 CCD掃描器(HC56II-TR)線路外層有脫落且刷讀條碼不太好刷，有執行校正仍異常....需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D191</t>
+  </si>
+  <si>
+    <t>2025-09-18 10:05:29</t>
+  </si>
+  <si>
+    <t>2025-09-18 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-18 12:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-19 14:05:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119008295
+換上8119012936</t>
+  </si>
+  <si>
+    <t>新莊昌平店</t>
+  </si>
+  <si>
+    <t>THILF04701</t>
+  </si>
+  <si>
+    <t>2025-09-18 11:18:47</t>
+  </si>
+  <si>
+    <t>2025-09-18 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-18 11:20:00</t>
+  </si>
+  <si>
+    <t>新莊棒球場</t>
+  </si>
+  <si>
+    <t>THILF03358</t>
+  </si>
+  <si>
+    <t>2025-09-18 11:34:07</t>
+  </si>
+  <si>
+    <t>2025-09-18 11:40:00</t>
+  </si>
+  <si>
+    <t>新莊輔園店</t>
+  </si>
+  <si>
+    <t>THILF03851</t>
+  </si>
+  <si>
+    <t>2025-09-18 13:11:21</t>
+  </si>
+  <si>
+    <t>2025-09-18 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-18 13:20:00</t>
   </si>
 </sst>
 </file>
@@ -2783,10 +2894,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK92"/>
+  <dimension ref="A1:AK97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC89" sqref="AC89"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10835,7 +10946,7 @@
       <c r="M92" s="4"/>
       <c r="N92" s="3"/>
       <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
+      <c r="P92" s="10"/>
       <c r="Q92" s="3" t="s">
         <v>744</v>
       </c>
@@ -10866,7 +10977,7 @@
       </c>
       <c r="AA92" s="3"/>
       <c r="AB92" s="3"/>
-      <c r="AC92" s="4" t="s">
+      <c r="AC92" s="10" t="s">
         <v>748</v>
       </c>
       <c r="AD92" s="3"/>
@@ -10879,6 +10990,435 @@
       <c r="AI92" s="3"/>
       <c r="AJ92" s="3"/>
       <c r="AK92" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="7">
+        <v>2025092373</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="K93" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L93" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M93" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N93" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O93" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P93" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="Q93" s="7" t="s">
+        <v>754</v>
+      </c>
+      <c r="R93" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T93" s="7">
+        <v>1</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V93" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="W93" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="X93" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="Y93" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="Z93" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC93" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="AD93" s="7"/>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="7"/>
+      <c r="AH93" s="7"/>
+      <c r="AI93" s="7"/>
+      <c r="AJ93" s="7"/>
+      <c r="AK93" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:37">
+      <c r="A94" s="3">
+        <v>92</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C94" s="3">
+        <v>2025092384</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L94" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N94" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O94" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P94" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="Q94" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="R94" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S94" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T94" s="3">
+        <v>1</v>
+      </c>
+      <c r="U94" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V94" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="W94" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="X94" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="Y94" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="Z94" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC94" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="AD94" s="3"/>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="3"/>
+      <c r="AG94" s="3"/>
+      <c r="AH94" s="3"/>
+      <c r="AI94" s="3"/>
+      <c r="AJ94" s="3"/>
+      <c r="AK94" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:37">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" s="7">
+        <v>2025092399</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7">
+        <v>4701</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="7"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="R95" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S95" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T95" s="7">
+        <v>1</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V95" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="W95" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="X95" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="Y95" s="7"/>
+      <c r="Z95" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA95" s="7"/>
+      <c r="AB95" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC95" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD95" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE95" s="7"/>
+      <c r="AF95" s="7"/>
+      <c r="AG95" s="7"/>
+      <c r="AH95" s="7"/>
+      <c r="AI95" s="7"/>
+      <c r="AJ95" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK95" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2025092404</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3">
+        <v>3358</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="R96" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S96" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T96" s="3">
+        <v>1</v>
+      </c>
+      <c r="U96" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V96" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="W96" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="X96" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC96" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD96" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE96" s="3"/>
+      <c r="AF96" s="3"/>
+      <c r="AG96" s="3"/>
+      <c r="AH96" s="3"/>
+      <c r="AI96" s="3"/>
+      <c r="AJ96" s="3"/>
+      <c r="AK96" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:37">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C97" s="7">
+        <v>2025092409</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7">
+        <v>3851</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="8"/>
+      <c r="Q97" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="R97" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T97" s="7">
+        <v>1</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V97" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="W97" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="X97" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC97" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD97" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="7"/>
+      <c r="AH97" s="7"/>
+      <c r="AI97" s="7"/>
+      <c r="AJ97" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK97" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09191636
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$98</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="785">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-18  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="794">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-19  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2481,6 +2481,35 @@
   </si>
   <si>
     <t>2025-09-18 13:20:00</t>
+  </si>
+  <si>
+    <t>13243114091801</t>
+  </si>
+  <si>
+    <t>2025-09-18 16:12:04</t>
+  </si>
+  <si>
+    <t>多張吃紙、卡紙</t>
+  </si>
+  <si>
+    <t>SC雷射印表機(M6600NW)-門市反應9/10更換設備後，頻繁發生卡紙異狀，都卡在滾輪裡面，碳粉也都漏的很誇張，都需慢慢手動清潔，門市需請工程師到店協助確認 PS.非24H營業門市，周一至周五0700~1900營業</t>
+  </si>
+  <si>
+    <t>2025-09-18 16:16:50</t>
+  </si>
+  <si>
+    <t>2025-09-19 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-19 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-19 20:16:00</t>
+  </si>
+  <si>
+    <t>更換印表機
+換上8103001960
+換下8103002250</t>
   </si>
 </sst>
 </file>
@@ -2894,10 +2923,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK97"/>
+  <dimension ref="A1:AK98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="AC95" sqref="AC95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11371,7 +11400,7 @@
       <c r="M97" s="8"/>
       <c r="N97" s="7"/>
       <c r="O97" s="8"/>
-      <c r="P97" s="8"/>
+      <c r="P97" s="9"/>
       <c r="Q97" s="7" t="s">
         <v>781</v>
       </c>
@@ -11404,7 +11433,7 @@
       <c r="AB97" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC97" s="8" t="s">
+      <c r="AC97" s="9" t="s">
         <v>272</v>
       </c>
       <c r="AD97" s="7" t="s">
@@ -11419,6 +11448,103 @@
         <v>60</v>
       </c>
       <c r="AK97" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:37">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2025092499</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F98" s="3">
+        <v>3243</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="N98" s="3">
+        <v>2701</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="P98" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="Q98" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T98" s="3">
+        <v>1</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V98" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="X98" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="Y98" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="Z98" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC98" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="AD98" s="3"/>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="3"/>
+      <c r="AG98" s="3"/>
+      <c r="AH98" s="3"/>
+      <c r="AI98" s="3"/>
+      <c r="AJ98" s="3"/>
+      <c r="AK98" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09221320
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$98</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$100</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="794">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-19  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="814">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-22  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2510,6 +2510,71 @@
     <t>更換印表機
 換上8103001960
 換下8103002250</t>
+  </si>
+  <si>
+    <t>E4341114091901</t>
+  </si>
+  <si>
+    <t>新莊莊美店</t>
+  </si>
+  <si>
+    <t>2025-09-19 09:29:39</t>
+  </si>
+  <si>
+    <t>F604</t>
+  </si>
+  <si>
+    <t>無電源反應</t>
+  </si>
+  <si>
+    <t>門市反應TM2多卡機(QP3000E)線路接觸不良常常螢幕會閃退，門市已有重插線路仍異常...須請台芝到店協助(電源接觸不良)</t>
+  </si>
+  <si>
+    <t>THILF04341</t>
+  </si>
+  <si>
+    <t>2025-09-19 09:49:11</t>
+  </si>
+  <si>
+    <t>2025-09-22 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 13:49:00</t>
+  </si>
+  <si>
+    <t>更換多卡機
+換上8183001984
+換下8183001961</t>
+  </si>
+  <si>
+    <t>14788114092101</t>
+  </si>
+  <si>
+    <t>2025-09-21 09:46:42</t>
+  </si>
+  <si>
+    <t>9/21 10:15 緊急叫修:門市反應無法開啟訂貨3.0及HISHOP，開啟後都會出現已取消瀏覽該網頁的白畫面，客服嘗試至最高權限執行Getnewhoshop，接收程式期間視窗顯示HI_SC-CheckUpdate已經停止運作，執行砍TMorder後跑接收作業時顯示HI_Paramrecv已經停止運作，再次開啟HISHOP仍顯示已取消瀏覽該網頁的白畫面，開啟訂貨3.0會顯示電腦系統繁忙中，請關閉其他程式後再試或重新開機，重啟SC仍異常，與通訊嘉芳確認需更換SC第一顆硬碟不備份還原..請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳務做到09/20，昨天只有使用TM1，與通訊嘉芳確認有收到09/20的銷售</t>
+  </si>
+  <si>
+    <t>2025-09-21 10:20:12</t>
+  </si>
+  <si>
+    <t>2025-09-21 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-21 14:40:00</t>
+  </si>
+  <si>
+    <t>2025-09-21 16:20:00</t>
+  </si>
+  <si>
+    <t>更換第一顆硬碟不備份還原
+並告知譚小姐更換硬碟注意事項
+SC = 20250805
+SC_Slave = 20250805</t>
   </si>
 </sst>
 </file>
@@ -2923,10 +2988,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK98"/>
+  <dimension ref="A1:AK100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC95" sqref="AC95"/>
+      <selection activeCell="AC97" sqref="AC97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11497,7 +11562,7 @@
       <c r="O98" s="4" t="s">
         <v>787</v>
       </c>
-      <c r="P98" s="4" t="s">
+      <c r="P98" s="10" t="s">
         <v>788</v>
       </c>
       <c r="Q98" s="3" t="s">
@@ -11534,7 +11599,7 @@
       <c r="AB98" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC98" s="4" t="s">
+      <c r="AC98" s="10" t="s">
         <v>793</v>
       </c>
       <c r="AD98" s="3"/>
@@ -11545,6 +11610,200 @@
       <c r="AI98" s="3"/>
       <c r="AJ98" s="3"/>
       <c r="AK98" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:37">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C99" s="7">
+        <v>2025092563</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>794</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F99" s="7">
+        <v>4341</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K99" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L99" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M99" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="N99" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="O99" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="P99" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="Q99" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T99" s="7">
+        <v>1</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V99" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="W99" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="Y99" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="Z99" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC99" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="AD99" s="7"/>
+      <c r="AE99" s="7"/>
+      <c r="AF99" s="7"/>
+      <c r="AG99" s="7"/>
+      <c r="AH99" s="7"/>
+      <c r="AI99" s="7"/>
+      <c r="AJ99" s="7"/>
+      <c r="AK99" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:37">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2025092791</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F100" s="3">
+        <v>4788</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L100" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M100" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N100" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O100" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P100" s="4" t="s">
+        <v>808</v>
+      </c>
+      <c r="Q100" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="R100" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T100" s="3">
+        <v>1</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V100" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="X100" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="Y100" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="Z100" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC100" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="AD100" s="3"/>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3"/>
+      <c r="AK100" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09221740
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$100</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$103</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="838">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-22  )</t>
   </si>
@@ -2550,6 +2550,69 @@
 換下8183001961</t>
   </si>
   <si>
+    <t>E3147114091901</t>
+  </si>
+  <si>
+    <t>北縣板明店</t>
+  </si>
+  <si>
+    <t>2025-09-19 14:40:06</t>
+  </si>
+  <si>
+    <t>列印效果異常</t>
+  </si>
+  <si>
+    <t>門市反應sc雷射印表機(M6600NW)列印一般商品卡列印未移，已確認列印設定有點選fit....須請台芝到店協助 請攜帶2台雷射印表機種(一台為不同型號)(列印商品卡格式跑掉)</t>
+  </si>
+  <si>
+    <t>THILF03147</t>
+  </si>
+  <si>
+    <t>2025-09-19 14:59:12</t>
+  </si>
+  <si>
+    <t>2025-09-22 15:25:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 15:55:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 18:59:00</t>
+  </si>
+  <si>
+    <t>驅動重新設定後正常</t>
+  </si>
+  <si>
+    <t>E2224114091901</t>
+  </si>
+  <si>
+    <t>2025-09-19 19:06:26</t>
+  </si>
+  <si>
+    <t>HL58</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET主機</t>
+  </si>
+  <si>
+    <t>門市告知MMK出現網路設定介面，已有點選1&gt;2確認網路設定連線正常且設定完成後再點選3重新開機,但重新開機後仍會跳回網路設定介面,ping60不通,已有重新開機仍無法排除....還請台芝到店協助(網路連線異常)</t>
+  </si>
+  <si>
+    <t>2025-09-19 19:25:30</t>
+  </si>
+  <si>
+    <t>2025-09-22 16:38:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 17:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 23:25:00</t>
+  </si>
+  <si>
+    <t>MMK更換硬碟</t>
+  </si>
+  <si>
     <t>14788114092101</t>
   </si>
   <si>
@@ -2575,6 +2638,15 @@
 並告知譚小姐更換硬碟注意事項
 SC = 20250805
 SC_Slave = 20250805</t>
+  </si>
+  <si>
+    <t>2025-09-22 16:14:43</t>
+  </si>
+  <si>
+    <t>2025-09-22 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-22 16:12:00</t>
   </si>
 </sst>
 </file>
@@ -2988,10 +3060,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK100"/>
+  <dimension ref="A1:AK103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC97" sqref="AC97"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11718,55 +11790,55 @@
         <v>38</v>
       </c>
       <c r="C100" s="3">
-        <v>2025092791</v>
+        <v>2025092717</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>806</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="F100" s="3">
-        <v>4788</v>
+        <v>3147</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>278</v>
+        <v>807</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>212</v>
+        <v>63</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="L100" s="3" t="s">
-        <v>297</v>
+        <v>452</v>
       </c>
       <c r="M100" s="4" t="s">
-        <v>298</v>
+        <v>453</v>
       </c>
       <c r="N100" s="3">
-        <v>2405</v>
+        <v>2705</v>
       </c>
       <c r="O100" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="P100" s="4" t="s">
-        <v>808</v>
+        <v>809</v>
+      </c>
+      <c r="P100" s="10" t="s">
+        <v>810</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>279</v>
+        <v>811</v>
       </c>
       <c r="R100" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S100" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="T100" s="3">
         <v>1</v>
@@ -11775,26 +11847,26 @@
         <v>53</v>
       </c>
       <c r="V100" s="3" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="W100" s="3" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="X100" s="3" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="Y100" s="3" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="Z100" s="3">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="AA100" s="3"/>
       <c r="AB100" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC100" s="4" t="s">
-        <v>813</v>
+      <c r="AC100" s="10" t="s">
+        <v>816</v>
       </c>
       <c r="AD100" s="3"/>
       <c r="AE100" s="3"/>
@@ -11804,6 +11876,277 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
       <c r="AK100" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2025092786</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="7">
+        <v>2224</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K101" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L101" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="N101" s="7">
+        <v>5804</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="P101" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q101" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="R101" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T101" s="7">
+        <v>1</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V101" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="W101" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y101" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="Z101" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC101" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="AD101" s="7"/>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="7"/>
+      <c r="AH101" s="7"/>
+      <c r="AI101" s="7"/>
+      <c r="AJ101" s="7"/>
+      <c r="AK101" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:37">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C102" s="3">
+        <v>2025092791</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F102" s="3">
+        <v>4788</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N102" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O102" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P102" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="Q102" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="R102" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T102" s="3">
+        <v>1</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V102" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="X102" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="Y102" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="Z102" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC102" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="AD102" s="3"/>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3"/>
+      <c r="AK102" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:37">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C103" s="7">
+        <v>2025092889</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7">
+        <v>3147</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="8"/>
+      <c r="P103" s="8"/>
+      <c r="Q103" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="R103" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T103" s="7">
+        <v>1</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V103" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="W103" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC103" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD103" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="7"/>
+      <c r="AG103" s="7"/>
+      <c r="AH103" s="7"/>
+      <c r="AI103" s="7"/>
+      <c r="AJ103" s="7"/>
+      <c r="AK103" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09240935
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$103</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$119</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="838">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-22  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="936">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-24  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2640,6 +2640,42 @@
 SC_Slave = 20250805</t>
   </si>
   <si>
+    <t>ED024114092201</t>
+  </si>
+  <si>
+    <t>D024</t>
+  </si>
+  <si>
+    <t>三重三民店</t>
+  </si>
+  <si>
+    <t>2025-09-22 08:59:46</t>
+  </si>
+  <si>
+    <t>當機或無畫面</t>
+  </si>
+  <si>
+    <t>性質交接:門市反應MMK 四代機上方廣告看板少1個螺絲...請台芝到店協助(Life-ET 上方文宣架 少一顆螺絲)</t>
+  </si>
+  <si>
+    <t>THILF0D024</t>
+  </si>
+  <si>
+    <t>2025-09-22 09:03:31</t>
+  </si>
+  <si>
+    <t>2025-09-23 10:21:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 10:51:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 13:03:00</t>
+  </si>
+  <si>
+    <t>補上螺帽*1</t>
+  </si>
+  <si>
     <t>2025-09-22 16:14:43</t>
   </si>
   <si>
@@ -2647,6 +2683,270 @@
   </si>
   <si>
     <t>2025-09-22 16:12:00</t>
+  </si>
+  <si>
+    <t>14698114092201</t>
+  </si>
+  <si>
+    <t>2025-09-22 18:38:42</t>
+  </si>
+  <si>
+    <t>門市反應TM2掃描槍(HC76-TR)刷讀條碼無反應，確認有亮燈有逼聲，VNC查看游標有在輸入顯示的位置，已執行掃槍校正後仍異常，需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-22 18:45:59</t>
+  </si>
+  <si>
+    <t>2025-09-23 09:34:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 10:04:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 22:46:00</t>
+  </si>
+  <si>
+    <t>門市測試掃槍正常，教導店員需點擊螢幕後可正常使用</t>
+  </si>
+  <si>
+    <t>1T110114092301</t>
+  </si>
+  <si>
+    <t>T110</t>
+  </si>
+  <si>
+    <t>五股訓練教室027401</t>
+  </si>
+  <si>
+    <t>2025-09-23 09:48:41</t>
+  </si>
+  <si>
+    <t>後勤楊小姐反應五股訓練中心2樓SC教室T110可正常開機，但無法連線E綱，公司也無法下撒現金帳資料，已有重新開機重新拔插hub線路仍異常，ping 10.231.100.110不通無法vnc....需請協助
+因報修人員楊小姐不在訓練店也不方便到店確認設備型號，楊小姐告知台芝工程師有定期保養和維修的人員應知道設備型號且今天下午也有到店保養的預定行程，另外請台芝到店前可在與楊小姐通知
+地址：新北市五股區五工六路28號2樓(2535五股五工店樓上)</t>
+  </si>
+  <si>
+    <t>THILF0T110</t>
+  </si>
+  <si>
+    <t>2025-09-23 10:09:05</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:15:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 14:09:00</t>
+  </si>
+  <si>
+    <t>重設網路</t>
+  </si>
+  <si>
+    <t>1T111114092301</t>
+  </si>
+  <si>
+    <t>T111</t>
+  </si>
+  <si>
+    <t>2025-09-23 09:49:24</t>
+  </si>
+  <si>
+    <t>後勤楊小姐反應五股訓練中心2樓SC教室T111經常性斷線和關機，導致無法每月如期可下撒現金帳帳資料，已有重新開機重新拔插hub線路仍異常，ping 10.231.100.111不通無法vnc....需請協助
+因報修人員楊小姐不在訓練店也不方便到店確認設備型號，楊小姐告知台芝工程師有定期保養和維修的人員應知道設備型號且今天下午也有到店保養的預定行程，另外請台芝到店前可在與楊小姐通知
+地址：新北市五股區五工六路28號2樓(2535五股五工店樓上)</t>
+  </si>
+  <si>
+    <t>THILF0T111</t>
+  </si>
+  <si>
+    <t>2025-09-23 10:09:25</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:00:00</t>
+  </si>
+  <si>
+    <t>更換cpu風扇</t>
+  </si>
+  <si>
+    <t>1T100114092301</t>
+  </si>
+  <si>
+    <t>T100</t>
+  </si>
+  <si>
+    <t>2025-09-23 09:50:17</t>
+  </si>
+  <si>
+    <t>滑鼠故障無作用</t>
+  </si>
+  <si>
+    <t>後勤楊小姐反應五股訓練中心2樓SC教室T100講師機滑鼠故障無作用....需請協助
+因報修人員楊小姐不在訓練店也不方便到店確認設備型號，楊小姐告知台芝工程師有定期保養和維修的人員應知道設備型號且今天下午也有到店保養的預定行程，另外請台芝到店前可在與楊小姐通知
+地址：新北市五股區五工六路28號2樓(2535五股五工店樓上)</t>
+  </si>
+  <si>
+    <t>THILF0T100</t>
+  </si>
+  <si>
+    <t>2025-09-23 10:09:41</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:00:00</t>
+  </si>
+  <si>
+    <t>更換滑鼠</t>
+  </si>
+  <si>
+    <t>淡水台電宿舍</t>
+  </si>
+  <si>
+    <t>THILF02897</t>
+  </si>
+  <si>
+    <t>2025-09-23 11:51:45</t>
+  </si>
+  <si>
+    <t>2025-09-23 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 11:51:00</t>
+  </si>
+  <si>
+    <t>北縣淡俊店</t>
+  </si>
+  <si>
+    <t>THILF02318</t>
+  </si>
+  <si>
+    <t>2025-09-23 12:45:34</t>
+  </si>
+  <si>
+    <t>2025-09-23 12:25:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 12:45:00</t>
+  </si>
+  <si>
+    <t>淡水莊園店</t>
+  </si>
+  <si>
+    <t>THILF04153</t>
+  </si>
+  <si>
+    <t>2025-09-23 13:21:34</t>
+  </si>
+  <si>
+    <t>2025-09-23 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 13:21:00</t>
+  </si>
+  <si>
+    <t>淡水新洲店</t>
+  </si>
+  <si>
+    <t>THILF04529</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:08:07</t>
+  </si>
+  <si>
+    <t>2025-09-23 13:45:00</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:07:00</t>
+  </si>
+  <si>
+    <t>淡水新市一</t>
+  </si>
+  <si>
+    <t>THILF04093</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:50:36</t>
+  </si>
+  <si>
+    <t>2025-09-23 14:50:00</t>
+  </si>
+  <si>
+    <t>淡水沙崙店</t>
+  </si>
+  <si>
+    <t>THILF04802</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:24:35</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:24:00</t>
+  </si>
+  <si>
+    <t>TT01</t>
+  </si>
+  <si>
+    <t>五股訓練教室</t>
+  </si>
+  <si>
+    <t>THILF0TT01</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:25:08</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:30:00</t>
+  </si>
+  <si>
+    <t>五股五工店</t>
+  </si>
+  <si>
+    <t>THILF02535</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:35:31</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:45:00</t>
+  </si>
+  <si>
+    <t>五股興珍店</t>
+  </si>
+  <si>
+    <t>THILF02691</t>
+  </si>
+  <si>
+    <t>2025-09-23 15:53:46</t>
+  </si>
+  <si>
+    <t>2025-09-23 16:00:00</t>
+  </si>
+  <si>
+    <t>五股產業園區</t>
+  </si>
+  <si>
+    <t>THILF02390</t>
+  </si>
+  <si>
+    <t>2025-09-23 16:13:29</t>
+  </si>
+  <si>
+    <t>2025-09-23 16:15:00</t>
+  </si>
+  <si>
+    <t>L516</t>
+  </si>
+  <si>
+    <t>車麗屋新莊店</t>
+  </si>
+  <si>
+    <t>THILF0L516</t>
+  </si>
+  <si>
+    <t>2025-09-23 16:35:40</t>
+  </si>
+  <si>
+    <t>2025-09-23 16:30:00</t>
   </si>
 </sst>
 </file>
@@ -3060,10 +3360,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK103"/>
+  <dimension ref="A1:AK119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A103" sqref="A103"/>
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12078,38 +12378,58 @@
         <v>101</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C103" s="7">
-        <v>2025092889</v>
-      </c>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-      <c r="F103" s="7">
-        <v>3147</v>
+        <v>2025092805</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>836</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>807</v>
+        <v>837</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I103" s="7"/>
-      <c r="J103" s="7"/>
-      <c r="K103" s="7"/>
-      <c r="L103" s="7"/>
-      <c r="M103" s="8"/>
-      <c r="N103" s="7"/>
-      <c r="O103" s="8"/>
-      <c r="P103" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="I103" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="J103" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K103" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L103" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="N103" s="7">
+        <v>5801</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>839</v>
+      </c>
+      <c r="P103" s="9" t="s">
+        <v>840</v>
+      </c>
       <c r="Q103" s="7" t="s">
-        <v>811</v>
+        <v>841</v>
       </c>
       <c r="R103" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S103" s="7" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="T103" s="7">
         <v>1</v>
@@ -12118,28 +12438,28 @@
         <v>53</v>
       </c>
       <c r="V103" s="7" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="W103" s="7" t="s">
-        <v>836</v>
+        <v>843</v>
       </c>
       <c r="X103" s="7" t="s">
-        <v>837</v>
-      </c>
-      <c r="Y103" s="7"/>
+        <v>844</v>
+      </c>
+      <c r="Y103" s="7" t="s">
+        <v>845</v>
+      </c>
       <c r="Z103" s="7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AA103" s="7"/>
       <c r="AB103" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC103" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD103" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC103" s="9" t="s">
+        <v>846</v>
+      </c>
+      <c r="AD103" s="7"/>
       <c r="AE103" s="7"/>
       <c r="AF103" s="7"/>
       <c r="AG103" s="7"/>
@@ -12147,6 +12467,1324 @@
       <c r="AI103" s="7"/>
       <c r="AJ103" s="7"/>
       <c r="AK103" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:37">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2025092889</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3">
+        <v>3147</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="10"/>
+      <c r="Q104" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="R104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S104" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="X104" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC104" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3"/>
+      <c r="AK104" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:37">
+      <c r="A105" s="7">
+        <v>103</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C105" s="7">
+        <v>2025092913</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F105" s="7">
+        <v>4698</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I105" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="J105" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K105" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L105" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N105" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P105" s="9" t="s">
+        <v>852</v>
+      </c>
+      <c r="Q105" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="R105" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T105" s="7">
+        <v>1</v>
+      </c>
+      <c r="U105" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V105" s="7" t="s">
+        <v>853</v>
+      </c>
+      <c r="W105" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="X105" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="Y105" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="Z105" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC105" s="9" t="s">
+        <v>857</v>
+      </c>
+      <c r="AD105" s="7"/>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="7"/>
+      <c r="AG105" s="7"/>
+      <c r="AH105" s="7"/>
+      <c r="AI105" s="7"/>
+      <c r="AJ105" s="7"/>
+      <c r="AK105" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:37">
+      <c r="A106" s="3">
+        <v>104</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="3">
+        <v>2025092924</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N106" s="3">
+        <v>2401</v>
+      </c>
+      <c r="O106" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="P106" s="10" t="s">
+        <v>862</v>
+      </c>
+      <c r="Q106" s="3" t="s">
+        <v>863</v>
+      </c>
+      <c r="R106" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S106" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T106" s="3">
+        <v>1</v>
+      </c>
+      <c r="U106" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V106" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="W106" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="X106" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="Y106" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="Z106" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC106" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="AD106" s="3"/>
+      <c r="AE106" s="3"/>
+      <c r="AF106" s="3"/>
+      <c r="AG106" s="3"/>
+      <c r="AH106" s="3"/>
+      <c r="AI106" s="3"/>
+      <c r="AJ106" s="3"/>
+      <c r="AK106" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:37">
+      <c r="A107" s="7">
+        <v>105</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="7">
+        <v>2025092925</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>869</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>860</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>871</v>
+      </c>
+      <c r="J107" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K107" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L107" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="M107" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="N107" s="7">
+        <v>2401</v>
+      </c>
+      <c r="O107" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="P107" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="Q107" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="R107" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T107" s="7">
+        <v>1</v>
+      </c>
+      <c r="U107" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V107" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="W107" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="X107" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="Y107" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="Z107" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC107" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="AD107" s="7"/>
+      <c r="AE107" s="7"/>
+      <c r="AF107" s="7"/>
+      <c r="AG107" s="7"/>
+      <c r="AH107" s="7"/>
+      <c r="AI107" s="7"/>
+      <c r="AJ107" s="7"/>
+      <c r="AK107" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:37">
+      <c r="A108" s="3">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="3">
+        <v>2025092926</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N108" s="3">
+        <v>2403</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="Q108" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="R108" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S108" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T108" s="3">
+        <v>1</v>
+      </c>
+      <c r="U108" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V108" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="W108" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="X108" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="Y108" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="Z108" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA108" s="3"/>
+      <c r="AB108" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC108" s="10" t="s">
+        <v>885</v>
+      </c>
+      <c r="AD108" s="3"/>
+      <c r="AE108" s="3"/>
+      <c r="AF108" s="3"/>
+      <c r="AG108" s="3"/>
+      <c r="AH108" s="3"/>
+      <c r="AI108" s="3"/>
+      <c r="AJ108" s="3"/>
+      <c r="AK108" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:37">
+      <c r="A109" s="7">
+        <v>107</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C109" s="7">
+        <v>2025092940</v>
+      </c>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7">
+        <v>2897</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="8"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="8"/>
+      <c r="P109" s="9"/>
+      <c r="Q109" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="R109" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T109" s="7">
+        <v>1</v>
+      </c>
+      <c r="U109" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V109" s="7" t="s">
+        <v>888</v>
+      </c>
+      <c r="W109" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="X109" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="Y109" s="7"/>
+      <c r="Z109" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC109" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD109" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE109" s="7"/>
+      <c r="AF109" s="7"/>
+      <c r="AG109" s="7"/>
+      <c r="AH109" s="7"/>
+      <c r="AI109" s="7"/>
+      <c r="AJ109" s="7"/>
+      <c r="AK109" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:37">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2025092957</v>
+      </c>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3">
+        <v>2318</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="10"/>
+      <c r="Q110" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T110" s="3">
+        <v>1</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="X110" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="Y110" s="3"/>
+      <c r="Z110" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC110" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD110" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE110" s="3"/>
+      <c r="AF110" s="3"/>
+      <c r="AG110" s="3"/>
+      <c r="AH110" s="3"/>
+      <c r="AI110" s="3"/>
+      <c r="AJ110" s="3"/>
+      <c r="AK110" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:37">
+      <c r="A111" s="7">
+        <v>109</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C111" s="7">
+        <v>2025092965</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7">
+        <v>4153</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="8"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="8"/>
+      <c r="P111" s="9"/>
+      <c r="Q111" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="R111" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T111" s="7">
+        <v>1</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V111" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="W111" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="X111" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="Y111" s="7"/>
+      <c r="Z111" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA111" s="7"/>
+      <c r="AB111" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC111" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD111" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE111" s="7"/>
+      <c r="AF111" s="7"/>
+      <c r="AG111" s="7"/>
+      <c r="AH111" s="7"/>
+      <c r="AI111" s="7"/>
+      <c r="AJ111" s="7"/>
+      <c r="AK111" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:37">
+      <c r="A112" s="3">
+        <v>110</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C112" s="3">
+        <v>2025092978</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3">
+        <v>4529</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="10"/>
+      <c r="Q112" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S112" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T112" s="3">
+        <v>1</v>
+      </c>
+      <c r="U112" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V112" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="X112" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="Y112" s="3"/>
+      <c r="Z112" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA112" s="3"/>
+      <c r="AB112" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC112" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD112" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE112" s="3"/>
+      <c r="AF112" s="3"/>
+      <c r="AG112" s="3"/>
+      <c r="AH112" s="3"/>
+      <c r="AI112" s="3"/>
+      <c r="AJ112" s="3"/>
+      <c r="AK112" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:37">
+      <c r="A113" s="7">
+        <v>111</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C113" s="7">
+        <v>2025092982</v>
+      </c>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7">
+        <v>4093</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="8"/>
+      <c r="N113" s="7"/>
+      <c r="O113" s="8"/>
+      <c r="P113" s="9"/>
+      <c r="Q113" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="R113" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T113" s="7">
+        <v>1</v>
+      </c>
+      <c r="U113" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V113" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="W113" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="X113" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="Y113" s="7"/>
+      <c r="Z113" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA113" s="7"/>
+      <c r="AB113" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC113" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD113" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE113" s="7"/>
+      <c r="AF113" s="7"/>
+      <c r="AG113" s="7"/>
+      <c r="AH113" s="7"/>
+      <c r="AI113" s="7"/>
+      <c r="AJ113" s="7"/>
+      <c r="AK113" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:37">
+      <c r="A114" s="3">
+        <v>112</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2025093011</v>
+      </c>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3">
+        <v>4802</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="10"/>
+      <c r="Q114" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S114" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T114" s="3">
+        <v>1</v>
+      </c>
+      <c r="U114" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="W114" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="X114" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="Y114" s="3"/>
+      <c r="Z114" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA114" s="3"/>
+      <c r="AB114" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC114" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD114" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE114" s="3"/>
+      <c r="AF114" s="3"/>
+      <c r="AG114" s="3"/>
+      <c r="AH114" s="3"/>
+      <c r="AI114" s="3"/>
+      <c r="AJ114" s="3"/>
+      <c r="AK114" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2025093012</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="8"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>918</v>
+      </c>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD115" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK115" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2025093040</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <v>2535</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3"/>
+      <c r="AK116" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2025093044</v>
+      </c>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7">
+        <v>2691</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>923</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="7"/>
+      <c r="O117" s="8"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>925</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>926</v>
+      </c>
+      <c r="Y117" s="7"/>
+      <c r="Z117" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD117" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK117" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2025093051</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3">
+        <v>2390</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD118" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE118" s="3"/>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK118" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2025093056</v>
+      </c>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>932</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="7"/>
+      <c r="O119" s="8"/>
+      <c r="P119" s="8"/>
+      <c r="Q119" s="7" t="s">
+        <v>933</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>935</v>
+      </c>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC119" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD119" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7"/>
+      <c r="AK119" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09241710
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$119</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$123</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="956">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-24  )</t>
   </si>
@@ -2814,6 +2814,42 @@
     <t>2025-09-23 11:51:00</t>
   </si>
   <si>
+    <t>14312114092301</t>
+  </si>
+  <si>
+    <t>三重文化北</t>
+  </si>
+  <si>
+    <t>2025-09-23 11:57:34</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)觸控異常鼠標亂點飄移，VNC查看鼠標飄移嚴重無法觸控校正重啟仍異常，主客顯未張貼文宣....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04312</t>
+  </si>
+  <si>
+    <t>2025-09-23 11:59:08</t>
+  </si>
+  <si>
+    <t>2025-09-24 09:18:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 09:48:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 15:59:00</t>
+  </si>
+  <si>
+    <t>取消修原因：門市告知今日操作正常，想先觀察，故此筆叫修取消</t>
+  </si>
+  <si>
+    <t>2025-09-24 11:28:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 11:58:00</t>
+  </si>
+  <si>
     <t>北縣淡俊店</t>
   </si>
   <si>
@@ -2947,6 +2983,30 @@
   </si>
   <si>
     <t>2025-09-23 16:30:00</t>
+  </si>
+  <si>
+    <t>蘆洲湧蓮店</t>
+  </si>
+  <si>
+    <t>THILF04218</t>
+  </si>
+  <si>
+    <t>2025-09-24 16:34:37</t>
+  </si>
+  <si>
+    <t>2025-09-24 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 16:36:53</t>
+  </si>
+  <si>
+    <t>2025-09-24 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-24 13:30:00</t>
   </si>
 </sst>
 </file>
@@ -3360,10 +3420,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK119"/>
+  <dimension ref="A1:AK123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13017,32 +13077,52 @@
         <v>108</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C110" s="3">
-        <v>2025092957</v>
-      </c>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
+        <v>2025092950</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F110" s="3">
-        <v>2318</v>
+        <v>4312</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="3"/>
-      <c r="L110" s="3"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="3"/>
-      <c r="O110" s="4"/>
-      <c r="P110" s="10"/>
+        <v>96</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N110" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O110" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P110" s="10" t="s">
+        <v>894</v>
+      </c>
       <c r="Q110" s="3" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="R110" s="3" t="s">
         <v>51</v>
@@ -13057,28 +13137,28 @@
         <v>53</v>
       </c>
       <c r="V110" s="3" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="X110" s="3" t="s">
-        <v>895</v>
-      </c>
-      <c r="Y110" s="3"/>
+        <v>898</v>
+      </c>
+      <c r="Y110" s="3" t="s">
+        <v>899</v>
+      </c>
       <c r="Z110" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA110" s="3"/>
       <c r="AB110" s="3" t="s">
-        <v>58</v>
+        <v>592</v>
       </c>
       <c r="AC110" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD110" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="AD110" s="3"/>
       <c r="AE110" s="3"/>
       <c r="AF110" s="3"/>
       <c r="AG110" s="3"/>
@@ -13094,32 +13174,52 @@
         <v>109</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="C111" s="7">
-        <v>2025092965</v>
-      </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
+        <v>2025092950</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F111" s="7">
-        <v>4153</v>
+        <v>4312</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="I111" s="7"/>
-      <c r="J111" s="7"/>
-      <c r="K111" s="7"/>
-      <c r="L111" s="7"/>
-      <c r="M111" s="8"/>
-      <c r="N111" s="7"/>
-      <c r="O111" s="8"/>
-      <c r="P111" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="I111" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M111" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N111" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P111" s="9" t="s">
+        <v>894</v>
+      </c>
       <c r="Q111" s="7" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="R111" s="7" t="s">
         <v>51</v>
@@ -13128,34 +13228,34 @@
         <v>52</v>
       </c>
       <c r="T111" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U111" s="7" t="s">
         <v>53</v>
       </c>
       <c r="V111" s="7" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="W111" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="X111" s="7" t="s">
+        <v>902</v>
+      </c>
+      <c r="Y111" s="7" t="s">
         <v>899</v>
       </c>
-      <c r="X111" s="7" t="s">
-        <v>900</v>
-      </c>
-      <c r="Y111" s="7"/>
       <c r="Z111" s="7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AA111" s="7"/>
       <c r="AB111" s="7" t="s">
-        <v>58</v>
+        <v>592</v>
       </c>
       <c r="AC111" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD111" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="AD111" s="7"/>
       <c r="AE111" s="7"/>
       <c r="AF111" s="7"/>
       <c r="AG111" s="7"/>
@@ -13174,15 +13274,15 @@
         <v>135</v>
       </c>
       <c r="C112" s="3">
-        <v>2025092978</v>
+        <v>2025092957</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3">
-        <v>4529</v>
+        <v>2318</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>212</v>
@@ -13196,7 +13296,7 @@
       <c r="O112" s="4"/>
       <c r="P112" s="10"/>
       <c r="Q112" s="3" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="R112" s="3" t="s">
         <v>51</v>
@@ -13211,17 +13311,17 @@
         <v>53</v>
       </c>
       <c r="V112" s="3" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="W112" s="3" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="X112" s="3" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="Y112" s="3"/>
       <c r="Z112" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA112" s="3"/>
       <c r="AB112" s="3" t="s">
@@ -13251,15 +13351,15 @@
         <v>135</v>
       </c>
       <c r="C113" s="7">
-        <v>2025092982</v>
+        <v>2025092965</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7">
-        <v>4093</v>
+        <v>4153</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>212</v>
@@ -13273,7 +13373,7 @@
       <c r="O113" s="8"/>
       <c r="P113" s="9"/>
       <c r="Q113" s="7" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="R113" s="7" t="s">
         <v>51</v>
@@ -13288,17 +13388,17 @@
         <v>53</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="W113" s="7" t="s">
-        <v>866</v>
+        <v>911</v>
       </c>
       <c r="X113" s="7" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="Y113" s="7"/>
       <c r="Z113" s="7">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA113" s="7"/>
       <c r="AB113" s="7" t="s">
@@ -13328,15 +13428,15 @@
         <v>135</v>
       </c>
       <c r="C114" s="3">
-        <v>2025093011</v>
+        <v>2025092978</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3">
-        <v>4802</v>
+        <v>4529</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>212</v>
@@ -13350,7 +13450,7 @@
       <c r="O114" s="4"/>
       <c r="P114" s="10"/>
       <c r="Q114" s="3" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="R114" s="3" t="s">
         <v>51</v>
@@ -13365,13 +13465,13 @@
         <v>53</v>
       </c>
       <c r="V114" s="3" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="W114" s="3" t="s">
-        <v>875</v>
+        <v>916</v>
       </c>
       <c r="X114" s="3" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="Y114" s="3"/>
       <c r="Z114" s="3">
@@ -13405,18 +13505,18 @@
         <v>135</v>
       </c>
       <c r="C115" s="7">
-        <v>2025093012</v>
+        <v>2025092982</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
-      <c r="F115" s="7" t="s">
-        <v>914</v>
+      <c r="F115" s="7">
+        <v>4093</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>137</v>
+        <v>212</v>
       </c>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
@@ -13427,13 +13527,13 @@
       <c r="O115" s="8"/>
       <c r="P115" s="9"/>
       <c r="Q115" s="7" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="R115" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S115" s="7" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="T115" s="7">
         <v>1</v>
@@ -13442,17 +13542,17 @@
         <v>53</v>
       </c>
       <c r="V115" s="7" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="W115" s="7" t="s">
-        <v>875</v>
+        <v>866</v>
       </c>
       <c r="X115" s="7" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="Y115" s="7"/>
       <c r="Z115" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA115" s="7"/>
       <c r="AB115" s="7" t="s">
@@ -13469,9 +13569,7 @@
       <c r="AG115" s="7"/>
       <c r="AH115" s="7"/>
       <c r="AI115" s="7"/>
-      <c r="AJ115" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ115" s="7"/>
       <c r="AK115" s="7" t="s">
         <v>60</v>
       </c>
@@ -13484,18 +13582,18 @@
         <v>135</v>
       </c>
       <c r="C116" s="3">
-        <v>2025093040</v>
+        <v>2025093011</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3">
-        <v>2535</v>
+        <v>4802</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>137</v>
+        <v>212</v>
       </c>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
@@ -13506,13 +13604,13 @@
       <c r="O116" s="4"/>
       <c r="P116" s="10"/>
       <c r="Q116" s="3" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="R116" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="T116" s="3">
         <v>1</v>
@@ -13521,24 +13619,24 @@
         <v>53</v>
       </c>
       <c r="V116" s="3" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="W116" s="3" t="s">
-        <v>918</v>
+        <v>875</v>
       </c>
       <c r="X116" s="3" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="Y116" s="3"/>
       <c r="Z116" s="3">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA116" s="3"/>
       <c r="AB116" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC116" s="10" t="s">
-        <v>272</v>
+        <v>141</v>
       </c>
       <c r="AD116" s="3" t="s">
         <v>60</v>
@@ -13561,15 +13659,15 @@
         <v>135</v>
       </c>
       <c r="C117" s="7">
-        <v>2025093044</v>
+        <v>2025093012</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
-      <c r="F117" s="7">
-        <v>2691</v>
+      <c r="F117" s="7" t="s">
+        <v>926</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>137</v>
@@ -13583,7 +13681,7 @@
       <c r="O117" s="8"/>
       <c r="P117" s="9"/>
       <c r="Q117" s="7" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="R117" s="7" t="s">
         <v>51</v>
@@ -13598,24 +13696,24 @@
         <v>53</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="W117" s="7" t="s">
-        <v>922</v>
+        <v>875</v>
       </c>
       <c r="X117" s="7" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="Y117" s="7"/>
       <c r="Z117" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA117" s="7"/>
       <c r="AB117" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC117" s="9" t="s">
-        <v>272</v>
+        <v>141</v>
       </c>
       <c r="AD117" s="7" t="s">
         <v>60</v>
@@ -13640,15 +13738,15 @@
         <v>135</v>
       </c>
       <c r="C118" s="3">
-        <v>2025093051</v>
+        <v>2025093040</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3">
-        <v>2390</v>
+        <v>2535</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>927</v>
+        <v>931</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>137</v>
@@ -13662,7 +13760,7 @@
       <c r="O118" s="4"/>
       <c r="P118" s="10"/>
       <c r="Q118" s="3" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="R118" s="3" t="s">
         <v>51</v>
@@ -13677,13 +13775,13 @@
         <v>53</v>
       </c>
       <c r="V118" s="3" t="s">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="W118" s="3" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="X118" s="3" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="Y118" s="3"/>
       <c r="Z118" s="3">
@@ -13704,9 +13802,7 @@
       <c r="AG118" s="3"/>
       <c r="AH118" s="3"/>
       <c r="AI118" s="3"/>
-      <c r="AJ118" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ118" s="3"/>
       <c r="AK118" s="3" t="s">
         <v>60</v>
       </c>
@@ -13719,18 +13815,18 @@
         <v>135</v>
       </c>
       <c r="C119" s="7">
-        <v>2025093056</v>
+        <v>2025093044</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
-      <c r="F119" s="7" t="s">
-        <v>931</v>
+      <c r="F119" s="7">
+        <v>2691</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
@@ -13739,9 +13835,9 @@
       <c r="M119" s="8"/>
       <c r="N119" s="7"/>
       <c r="O119" s="8"/>
-      <c r="P119" s="8"/>
+      <c r="P119" s="9"/>
       <c r="Q119" s="7" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="R119" s="7" t="s">
         <v>51</v>
@@ -13756,13 +13852,13 @@
         <v>53</v>
       </c>
       <c r="V119" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="W119" s="7" t="s">
         <v>934</v>
       </c>
-      <c r="W119" s="7" t="s">
-        <v>930</v>
-      </c>
       <c r="X119" s="7" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Y119" s="7"/>
       <c r="Z119" s="7">
@@ -13772,8 +13868,8 @@
       <c r="AB119" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC119" s="8" t="s">
-        <v>141</v>
+      <c r="AC119" s="9" t="s">
+        <v>272</v>
       </c>
       <c r="AD119" s="7" t="s">
         <v>60</v>
@@ -13783,8 +13879,320 @@
       <c r="AG119" s="7"/>
       <c r="AH119" s="7"/>
       <c r="AI119" s="7"/>
-      <c r="AJ119" s="7"/>
+      <c r="AJ119" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AK119" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2025093051</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>2390</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC120" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE120" s="3"/>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK120" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:37">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C121" s="7">
+        <v>2025093056</v>
+      </c>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>944</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="7"/>
+      <c r="O121" s="8"/>
+      <c r="P121" s="9"/>
+      <c r="Q121" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="R121" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="T121" s="7">
+        <v>1</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="W121" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="X121" s="7" t="s">
+        <v>947</v>
+      </c>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC121" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD121" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7"/>
+      <c r="AK121" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2025093197</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <v>4218</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC122" s="10" t="s">
+        <v>748</v>
+      </c>
+      <c r="AD122" s="3"/>
+      <c r="AE122" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3"/>
+      <c r="AK122" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2025093202</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7">
+        <v>4218</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>948</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="8"/>
+      <c r="Q123" s="7" t="s">
+        <v>949</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>954</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC123" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD123" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09260849
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$123</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$133</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="956">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-24  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1015">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-26  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3007,6 +3007,189 @@
   </si>
   <si>
     <t>2025-09-24 13:30:00</t>
+  </si>
+  <si>
+    <t>D072</t>
+  </si>
+  <si>
+    <t>板橋僑福店</t>
+  </si>
+  <si>
+    <t>THILF0D072</t>
+  </si>
+  <si>
+    <t>2025-09-25 13:45:55</t>
+  </si>
+  <si>
+    <t>2025-09-25 13:15:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 13:36:00</t>
+  </si>
+  <si>
+    <t>板橋板好店</t>
+  </si>
+  <si>
+    <t>THILF03183</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:08:40</t>
+  </si>
+  <si>
+    <t>2025-09-25 13:45:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:03:00</t>
+  </si>
+  <si>
+    <t>板橋藝文店</t>
+  </si>
+  <si>
+    <t>THILF04983</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:31:34</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:29:00</t>
+  </si>
+  <si>
+    <t>板橋湳雅夜市</t>
+  </si>
+  <si>
+    <t>THILF02995</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:03:21</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:39:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:00:00</t>
+  </si>
+  <si>
+    <t>13818114092502</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:00:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sc(SHUTTLE6S):門市TM1.2清帳時畫面卡在帳條列印中都無反應卡了10分鐘以上，確認帳條已有印出。hipos回覆:查看TM1、TM2清帳成功，協助調整入帳日後，執行版本更新顯示與SC連線失敗，重啟SC.Server無法開啟，判斷為硬碟損毀，煩請轉派台芝到店更換硬碟。通訊健誌副理告知為第二顆硬碟有問題...請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+與門市確認帳務做到09/25，與通訊健誌副理確認有收到09/25的銷售																																
+</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:11:12</t>
+  </si>
+  <si>
+    <t>2025-09-25 16:23:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 16:53:00</t>
+  </si>
+  <si>
+    <t>2025-09-26 19:11:00</t>
+  </si>
+  <si>
+    <t>更換SC第二顆硬碟無備份還原
+SC_Slave = 20250805</t>
+  </si>
+  <si>
+    <t>13551114092501</t>
+  </si>
+  <si>
+    <t>板橋板豐店</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:16:44</t>
+  </si>
+  <si>
+    <t>門市反應TM1CCD掃描器(HC56IITR、HC76TR)刷讀所有條碼都感應不良，已有執行掃描器校正仍無改善..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03551</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:18:54</t>
+  </si>
+  <si>
+    <t>2025-09-25 14:58:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:28:00</t>
+  </si>
+  <si>
+    <t>2025-09-26 19:18:00</t>
+  </si>
+  <si>
+    <t>報錯櫃號，取消報修</t>
+  </si>
+  <si>
+    <t>13551114092502</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:23:05</t>
+  </si>
+  <si>
+    <t>門市反應TM2 CCD掃描器(HC56IITR、HC76TR)刷讀所有條碼都感應不良，已有執行掃描器校正仍無改善..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:23:47</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:27:00</t>
+  </si>
+  <si>
+    <t>2025-09-26 19:23:00</t>
+  </si>
+  <si>
+    <t>更換76掃槍
+換上：8119012710
+換下：8119008647</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:33:02</t>
+  </si>
+  <si>
+    <t>北縣板莊店</t>
+  </si>
+  <si>
+    <t>THILF02154</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:49:10</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:35:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:46:00</t>
+  </si>
+  <si>
+    <t>L501</t>
+  </si>
+  <si>
+    <t>車麗屋板橋店</t>
+  </si>
+  <si>
+    <t>THILF0L501</t>
+  </si>
+  <si>
+    <t>2025-09-25 16:08:45</t>
+  </si>
+  <si>
+    <t>2025-09-25 15:55:00</t>
+  </si>
+  <si>
+    <t>2025-09-25 16:05:00</t>
   </si>
 </sst>
 </file>
@@ -3420,10 +3603,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK123"/>
+  <dimension ref="A1:AK133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A123" sqref="A123"/>
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14147,7 +14330,7 @@
       <c r="M123" s="8"/>
       <c r="N123" s="7"/>
       <c r="O123" s="8"/>
-      <c r="P123" s="8"/>
+      <c r="P123" s="9"/>
       <c r="Q123" s="7" t="s">
         <v>949</v>
       </c>
@@ -14180,7 +14363,7 @@
       <c r="AB123" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC123" s="8" t="s">
+      <c r="AC123" s="9" t="s">
         <v>141</v>
       </c>
       <c r="AD123" s="7" t="s">
@@ -14193,6 +14376,834 @@
       <c r="AI123" s="7"/>
       <c r="AJ123" s="7"/>
       <c r="AK123" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2025093266</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="Y124" s="3"/>
+      <c r="Z124" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD124" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3"/>
+      <c r="AK124" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2025093274</v>
+      </c>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7">
+        <v>3183</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I125" s="7"/>
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+      <c r="L125" s="7"/>
+      <c r="M125" s="8"/>
+      <c r="N125" s="7"/>
+      <c r="O125" s="8"/>
+      <c r="P125" s="9"/>
+      <c r="Q125" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>966</v>
+      </c>
+      <c r="Y125" s="7"/>
+      <c r="Z125" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD125" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7"/>
+      <c r="AK125" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2025093282</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3">
+        <v>4983</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="Y126" s="3"/>
+      <c r="Z126" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC126" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD126" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3"/>
+      <c r="AK126" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2025093289</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7">
+        <v>2995</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD127" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE127" s="7"/>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7"/>
+      <c r="AK127" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2025093295</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F128" s="3">
+        <v>3818</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L128" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M128" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N128" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O128" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P128" s="10" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q128" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="Y128" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="Z128" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC128" s="10" t="s">
+        <v>984</v>
+      </c>
+      <c r="AD128" s="3"/>
+      <c r="AE128" s="3"/>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3"/>
+      <c r="AK128" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:37">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C129" s="7">
+        <v>2025093305</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>985</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F129" s="7">
+        <v>3551</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I129" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L129" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M129" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N129" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O129" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P129" s="9" t="s">
+        <v>988</v>
+      </c>
+      <c r="Q129" s="7" t="s">
+        <v>989</v>
+      </c>
+      <c r="R129" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S129" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T129" s="7">
+        <v>1</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V129" s="7" t="s">
+        <v>990</v>
+      </c>
+      <c r="W129" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="X129" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="Y129" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="Z129" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>994</v>
+      </c>
+      <c r="AD129" s="7"/>
+      <c r="AE129" s="7"/>
+      <c r="AF129" s="7"/>
+      <c r="AG129" s="7"/>
+      <c r="AH129" s="7"/>
+      <c r="AI129" s="7"/>
+      <c r="AJ129" s="7"/>
+      <c r="AK129" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:37">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2025093307</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F130" s="3">
+        <v>3551</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L130" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M130" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N130" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O130" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P130" s="10" t="s">
+        <v>997</v>
+      </c>
+      <c r="Q130" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T130" s="3">
+        <v>1</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="W130" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Y130" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="Z130" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC130" s="10" t="s">
+        <v>1002</v>
+      </c>
+      <c r="AD130" s="3"/>
+      <c r="AE130" s="3"/>
+      <c r="AF130" s="3"/>
+      <c r="AG130" s="3"/>
+      <c r="AH130" s="3"/>
+      <c r="AI130" s="3"/>
+      <c r="AJ130" s="3"/>
+      <c r="AK130" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:37">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C131" s="7">
+        <v>2025093308</v>
+      </c>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7">
+        <v>3551</v>
+      </c>
+      <c r="G131" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I131" s="7"/>
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+      <c r="L131" s="7"/>
+      <c r="M131" s="8"/>
+      <c r="N131" s="7"/>
+      <c r="O131" s="8"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="7" t="s">
+        <v>989</v>
+      </c>
+      <c r="R131" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S131" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T131" s="7">
+        <v>1</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V131" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="W131" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="X131" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Y131" s="7"/>
+      <c r="Z131" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC131" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD131" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7"/>
+    </row>
+    <row r="132" spans="1:37">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2025093318</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3">
+        <v>2154</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T132" s="3">
+        <v>1</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="W132" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="X132" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Y132" s="3"/>
+      <c r="Z132" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA132" s="3"/>
+      <c r="AB132" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC132" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD132" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE132" s="3"/>
+      <c r="AF132" s="3"/>
+      <c r="AG132" s="3"/>
+      <c r="AH132" s="3"/>
+      <c r="AI132" s="3"/>
+      <c r="AJ132" s="3"/>
+      <c r="AK132" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2025093321</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="7"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="Q133" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="R133" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S133" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T133" s="7">
+        <v>1</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="W133" s="7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="X133" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC133" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD133" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE133" s="7"/>
+      <c r="AF133" s="7"/>
+      <c r="AG133" s="7"/>
+      <c r="AH133" s="7"/>
+      <c r="AI133" s="7"/>
+      <c r="AJ133" s="7"/>
+      <c r="AK133" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 09301404
</commit_message>
<xml_diff>
--- a/IM/202509_HL_Maintain_Report.xlsx
+++ b/IM/202509_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$133</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$137</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1015">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-26  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1047">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202509   (  製表日期:2025-09-30  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3190,6 +3190,111 @@
   </si>
   <si>
     <t>2025-09-25 16:05:00</t>
+  </si>
+  <si>
+    <t>1D609114092601</t>
+  </si>
+  <si>
+    <t>2025-09-26 09:09:07</t>
+  </si>
+  <si>
+    <t>D301</t>
+  </si>
+  <si>
+    <t>發票切刀卡紙，切紙不正常</t>
+  </si>
+  <si>
+    <t>門市反應TM1發票機(BSC10II)近期常發生卡紙的狀況一天會連續很多次，門市已有重裝紙捲重開機仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-26 09:10:21</t>
+  </si>
+  <si>
+    <t>2025-09-26 13:16:00</t>
+  </si>
+  <si>
+    <t>2025-09-26 13:46:00</t>
+  </si>
+  <si>
+    <t>2025-09-30 13:10:00</t>
+  </si>
+  <si>
+    <t>1D609114092602</t>
+  </si>
+  <si>
+    <t>2025-09-26 11:58:47</t>
+  </si>
+  <si>
+    <t>D305</t>
+  </si>
+  <si>
+    <t>9/26 11:58 總公司明翰來電啟動緊急叫修:門市反應TM1發票機(BSC10II)近期常發生卡紙的狀況一天會連續很多次，門市已有重裝紙捲重開機仍異常，後續再次進線告知已完全無電源反應，確認線路無鬆脫按壓電源鍵仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-26 12:02:23</t>
+  </si>
+  <si>
+    <t>2025-09-26 18:02:00</t>
+  </si>
+  <si>
+    <t>到場後測試正常，門市表示清帳後才發生異常
+更換發票機
+換上：8155004451
+換下：8155005445</t>
+  </si>
+  <si>
+    <t>13818114092701</t>
+  </si>
+  <si>
+    <t>2025-09-27 10:25:28</t>
+  </si>
+  <si>
+    <t>09/27 10:30 啟動緊急叫修:hub(DES1210-28)門市反應店內網路斷線ping全店僅90通，請門市查看hub、peplink、adsl皆有過電，已將hub、peplink、adsl重啟網路仍異常，peplink只亮status，請門市查看hub 13port未亮燈，請門市將13port插到其他孔洞皆未亮燈網路也未恢復....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-09-27 10:30:36</t>
+  </si>
+  <si>
+    <t>2025-09-27 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-27 15:10:00</t>
+  </si>
+  <si>
+    <t>2025-09-27 16:30:00</t>
+  </si>
+  <si>
+    <t>中華主線13pirt網路線損壞，已找尋替代線路
+數據機架設櫃子中易熱當
+更換HUB
+換上：8107005218
+換下：8107003337</t>
+  </si>
+  <si>
+    <t>14698114092701</t>
+  </si>
+  <si>
+    <t>2025-09-27 11:32:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/27 11:44 萊爾富百大門市啟動緊急叫修:門市反應TM1(TCX800)清帳後呈現黑底英文字，帳條有出，已有將線路拔除休息10分鐘後再開機畫面仍異常，電源燈亮藍燈，PING80不通無法VNC...請台芝到店協助
+已與門市確認09/27已清帳，清帳後畫面黑底英文字，尚未有交易。PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+</t>
+  </si>
+  <si>
+    <t>2025-09-27 11:46:48</t>
+  </si>
+  <si>
+    <t>2025-09-27 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-27 15:29:00</t>
+  </si>
+  <si>
+    <t>2025-09-27 17:46:00</t>
+  </si>
+  <si>
+    <t>更換第一顆硬碟不備份還原完成</t>
   </si>
 </sst>
 </file>
@@ -3603,10 +3708,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK133"/>
+  <dimension ref="A1:AK137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A133" sqref="A133"/>
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15158,7 +15263,7 @@
       <c r="M133" s="8"/>
       <c r="N133" s="7"/>
       <c r="O133" s="8"/>
-      <c r="P133" s="8"/>
+      <c r="P133" s="9"/>
       <c r="Q133" s="7" t="s">
         <v>1011</v>
       </c>
@@ -15191,7 +15296,7 @@
       <c r="AB133" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC133" s="8" t="s">
+      <c r="AC133" s="9" t="s">
         <v>141</v>
       </c>
       <c r="AD133" s="7" t="s">
@@ -15204,6 +15309,394 @@
       <c r="AI133" s="7"/>
       <c r="AJ133" s="7"/>
       <c r="AK133" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2025093347</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M134" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N134" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="O134" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P134" s="10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="Q134" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T134" s="3">
+        <v>1</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="W134" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="X134" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Y134" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="Z134" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA134" s="3"/>
+      <c r="AB134" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC134" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD134" s="3"/>
+      <c r="AE134" s="3"/>
+      <c r="AF134" s="3"/>
+      <c r="AG134" s="3"/>
+      <c r="AH134" s="3"/>
+      <c r="AI134" s="3"/>
+      <c r="AJ134" s="3"/>
+      <c r="AK134" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:37">
+      <c r="A135" s="7">
+        <v>133</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C135" s="7">
+        <v>2025093389</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I135" s="7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K135" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L135" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M135" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N135" s="7" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O135" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="P135" s="9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Q135" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="R135" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S135" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T135" s="7">
+        <v>1</v>
+      </c>
+      <c r="U135" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V135" s="7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="W135" s="7" t="s">
+        <v>1021</v>
+      </c>
+      <c r="X135" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Y135" s="7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Z135" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA135" s="7"/>
+      <c r="AB135" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC135" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="AD135" s="7"/>
+      <c r="AE135" s="7"/>
+      <c r="AF135" s="7"/>
+      <c r="AG135" s="7"/>
+      <c r="AH135" s="7"/>
+      <c r="AI135" s="7"/>
+      <c r="AJ135" s="7"/>
+      <c r="AK135" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:37">
+      <c r="A136" s="3">
+        <v>134</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C136" s="3">
+        <v>2025093482</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F136" s="3">
+        <v>3818</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="M136" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="N136" s="3">
+        <v>3402</v>
+      </c>
+      <c r="O136" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="P136" s="10" t="s">
+        <v>1033</v>
+      </c>
+      <c r="Q136" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="R136" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S136" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T136" s="3">
+        <v>1</v>
+      </c>
+      <c r="U136" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V136" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="W136" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="X136" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="Y136" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="Z136" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AA136" s="3"/>
+      <c r="AB136" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC136" s="10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="AD136" s="3"/>
+      <c r="AE136" s="3"/>
+      <c r="AF136" s="3"/>
+      <c r="AG136" s="3"/>
+      <c r="AH136" s="3"/>
+      <c r="AI136" s="3"/>
+      <c r="AJ136" s="3"/>
+      <c r="AK136" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:37">
+      <c r="A137" s="7">
+        <v>135</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="7">
+        <v>2025093483</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F137" s="7">
+        <v>4698</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I137" s="7" t="s">
+        <v>1040</v>
+      </c>
+      <c r="J137" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K137" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L137" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M137" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N137" s="7">
+        <v>2301</v>
+      </c>
+      <c r="O137" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="P137" s="8" t="s">
+        <v>1041</v>
+      </c>
+      <c r="Q137" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="R137" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S137" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T137" s="7">
+        <v>1</v>
+      </c>
+      <c r="U137" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V137" s="7" t="s">
+        <v>1042</v>
+      </c>
+      <c r="W137" s="7" t="s">
+        <v>1043</v>
+      </c>
+      <c r="X137" s="7" t="s">
+        <v>1044</v>
+      </c>
+      <c r="Y137" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="Z137" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC137" s="8" t="s">
+        <v>1046</v>
+      </c>
+      <c r="AD137" s="7"/>
+      <c r="AE137" s="7"/>
+      <c r="AF137" s="7"/>
+      <c r="AG137" s="7"/>
+      <c r="AH137" s="7"/>
+      <c r="AI137" s="7"/>
+      <c r="AJ137" s="7"/>
+      <c r="AK137" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>